<commit_message>
cahier de test fini
</commit_message>
<xml_diff>
--- a/annexes/Cahier_de_test.xlsx
+++ b/annexes/Cahier_de_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\rosetta\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47640E5-1816-4022-9DC7-565B2CA4A3B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3108A-12CC-44C2-B5F2-4C2648A018D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="332">
   <si>
     <t>Code</t>
   </si>
@@ -180,9 +180,6 @@
     <t>En tant qu'utilisateur je souhaite pouvoir me déconnecter</t>
   </si>
   <si>
-    <t>ExiWebAccueil4</t>
-  </si>
-  <si>
     <t>En tant qu'utilisateur je souhaite avoir accès via un menu aux pages devis, clients et scénarios</t>
   </si>
   <si>
@@ -312,19 +309,10 @@
     <t>En tant qu'utilisateur je souhaite pouvoir créer un devis</t>
   </si>
   <si>
-    <t>En tant qu'utilisateur je souhaite pouvoir consulter la liste des clients ainsi que mon calendrier</t>
-  </si>
-  <si>
-    <t>En tant qu'utilisateur je souhaite pouvoir consulter les derniers devis enregistrées</t>
-  </si>
-  <si>
     <t xml:space="preserve">En tant que utilisateur je souhaite pouvoir modifier une données </t>
   </si>
   <si>
     <t xml:space="preserve">En tant que utilisateur je souhaite pouvoir supprimer une données </t>
-  </si>
-  <si>
-    <t xml:space="preserve">En tant que utilisateur je souhaite pouvoir récolter des données </t>
   </si>
   <si>
     <t xml:space="preserve">En tant que utilisateur je souhaite pouvoir insérer des données </t>
@@ -923,12 +911,218 @@
   <si>
     <t>État</t>
   </si>
+  <si>
+    <t>Saisir login et mdp attribué à Thierry H</t>
+  </si>
+  <si>
+    <t>Se déconnecter</t>
+  </si>
+  <si>
+    <t>ExiWeb1 T1</t>
+  </si>
+  <si>
+    <t>ExiWeb1 T2</t>
+  </si>
+  <si>
+    <t>Mauvaise saisie des login</t>
+  </si>
+  <si>
+    <t>Affichage message d'erreur</t>
+  </si>
+  <si>
+    <t>ExiWebAccueil1 T</t>
+  </si>
+  <si>
+    <t>Être connecté --&gt; affichage des onglets client / devis / scénario</t>
+  </si>
+  <si>
+    <t>Être déconnecté --&gt; Absence des onglets client / devis / scénario</t>
+  </si>
+  <si>
+    <t>ExiWebAccueil2 T</t>
+  </si>
+  <si>
+    <t>En tant qu'utilisateur je souhaite pouvoir consulter mon calendrier</t>
+  </si>
+  <si>
+    <t>Faible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Affichage du calendrier </t>
+  </si>
+  <si>
+    <t>Consulter le calendrier</t>
+  </si>
+  <si>
+    <t>ExiWebAccueil3 T</t>
+  </si>
+  <si>
+    <t>Accèder le menu aux pages devis, clients et scénarios (URL : https://www..../client, https://www..../devis, https://www..../scénario)</t>
+  </si>
+  <si>
+    <t>Affichage des différentes pages (Client, Devis, Scénario)</t>
+  </si>
+  <si>
+    <t>Affichage du client dans la liste de client</t>
+  </si>
+  <si>
+    <t>ExiWebClient3 T1</t>
+  </si>
+  <si>
+    <t>ExiWebClient3 T2</t>
+  </si>
+  <si>
+    <t>Créer un client vide</t>
+  </si>
+  <si>
+    <t>ExiWebClient3 T3</t>
+  </si>
+  <si>
+    <t>Créer un client avec des infos syntaxiquement non valide (ex: prénom: Jean -&gt; X Æ A-12)</t>
+  </si>
+  <si>
+    <t>ExiWebClient1 T1</t>
+  </si>
+  <si>
+    <t>ExiWebClient1 T2</t>
+  </si>
+  <si>
+    <t>ExiWebClient2 T1</t>
+  </si>
+  <si>
+    <t>ExiWebClient2 T2</t>
+  </si>
+  <si>
+    <t>ExiWebClient2 T3</t>
+  </si>
+  <si>
+    <t>Rechercher n'importe quel client existant</t>
+  </si>
+  <si>
+    <t>ExiWebClient4 T</t>
+  </si>
+  <si>
+    <t>ExiWebClient5 T</t>
+  </si>
+  <si>
+    <t>ExiWebClient6 T</t>
+  </si>
+  <si>
+    <t>ExiWebClient7 T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insérer des données </t>
+  </si>
+  <si>
+    <t>Test OK</t>
+  </si>
+  <si>
+    <t>ExiApi1 T1</t>
+  </si>
+  <si>
+    <t>ExiApi1 T2</t>
+  </si>
+  <si>
+    <t>Insérer des données syntaxiquement invalide</t>
+  </si>
+  <si>
+    <t>Affichage de ses données dans la base de données</t>
+  </si>
+  <si>
+    <t>Affichage d'un message d'erreur et non insertion des données</t>
+  </si>
+  <si>
+    <t>ExiApi1 T3</t>
+  </si>
+  <si>
+    <t>Insérer des données vide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En tant que utilisateur je souhaite pouvoir récupérer des données </t>
+  </si>
+  <si>
+    <t>ExiApi2 T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récupérer des données </t>
+  </si>
+  <si>
+    <t>Affichage des données selectionnées</t>
+  </si>
+  <si>
+    <t>Modifier une donnée</t>
+  </si>
+  <si>
+    <t>Modification de la donnée effectué</t>
+  </si>
+  <si>
+    <t>ExiApi3 T1</t>
+  </si>
+  <si>
+    <t>ExiApi3 T2</t>
+  </si>
+  <si>
+    <t>ExiApi3 T3</t>
+  </si>
+  <si>
+    <t>Modifier les données en mettant un chaine de caractère vide aux champs d'entrée obligatoire</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Modifier les données et remplacer une donnée par une donnée syntaxiquement non valide (ex: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prénom</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Jean -&gt; X Æ A-12)</t>
+    </r>
+  </si>
+  <si>
+    <t>ExiApi4 T1</t>
+  </si>
+  <si>
+    <t>Absence de la donnée supprimer dans la base de données</t>
+  </si>
+  <si>
+    <t>ExiApi4 T2</t>
+  </si>
+  <si>
+    <t>Suprimer une donnée non existante</t>
+  </si>
+  <si>
+    <t>Supprimer une donnée</t>
+  </si>
+  <si>
+    <t>Synchroniser mes données</t>
+  </si>
+  <si>
+    <t>ExiApi5 T</t>
+  </si>
+  <si>
+    <t>Synchronisation des donnée entre la tablette et le site web</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -988,8 +1182,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1032,8 +1233,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1210,11 +1417,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1254,7 +1476,31 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1269,37 +1515,53 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1621,27 +1883,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D569B6-B3CB-4EA1-907F-9E75FD9F6494}">
-  <dimension ref="A1:K60"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="112.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="88.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="32" t="s">
-        <v>142</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
+      <c r="B1" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -1649,620 +1912,620 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="34" t="s">
-        <v>272</v>
+      <c r="B4" s="26" t="s">
+        <v>268</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" s="26" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="34" t="s">
-        <v>274</v>
+      <c r="F4" s="26" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="35"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="49"/>
       <c r="G5" s="8"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="G6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="30" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D7" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="C6" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="36" t="s">
+      <c r="E7" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="F7" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="F6" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="40" t="s">
-        <v>144</v>
-      </c>
-      <c r="C7" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>147</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="F7" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
-        <v>150</v>
-      </c>
-      <c r="C8" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="E8" s="36" t="s">
+      <c r="C10" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="F8" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="D9" s="37" t="s">
+      <c r="E10" s="30" t="s">
         <v>155</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="F10" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="F9" s="43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="C11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D10" s="40" t="s">
+      <c r="E11" s="27" t="s">
         <v>158</v>
       </c>
-      <c r="E10" s="40" t="s">
+      <c r="F11" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="30" t="s">
         <v>159</v>
       </c>
-      <c r="F10" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="C12" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>160</v>
       </c>
-      <c r="C11" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>161</v>
-      </c>
-      <c r="E11" s="36" t="s">
-        <v>162</v>
-      </c>
-      <c r="F11" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
-        <v>163</v>
-      </c>
-      <c r="C12" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>159</v>
-      </c>
-      <c r="F12" s="42" t="s">
-        <v>148</v>
+      <c r="E12" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
-      <c r="B13" s="36" t="s">
-        <v>213</v>
+      <c r="B13" s="27" t="s">
+        <v>209</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="F13" s="39" t="s">
-        <v>148</v>
+        <v>183</v>
+      </c>
+      <c r="F13" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
-      <c r="B14" s="36" t="s">
-        <v>214</v>
+      <c r="B14" s="27" t="s">
+        <v>210</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F14" s="39" t="s">
-        <v>148</v>
+        <v>163</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
-      <c r="B15" s="36" t="s">
-        <v>215</v>
+      <c r="B15" s="27" t="s">
+        <v>211</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="F15" s="39" t="s">
-        <v>148</v>
+        <v>165</v>
+      </c>
+      <c r="F15" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
-      <c r="B16" s="36" t="s">
-        <v>216</v>
+      <c r="B16" s="27" t="s">
+        <v>212</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="F16" s="39" t="s">
-        <v>148</v>
+        <v>167</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="44"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="26"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="36" t="s">
-        <v>172</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="36" t="s">
-        <v>173</v>
-      </c>
-      <c r="E18" s="36" t="s">
-        <v>174</v>
-      </c>
-      <c r="F18" s="41" t="s">
-        <v>148</v>
+      <c r="B18" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F18" s="50" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="40" t="s">
-        <v>175</v>
-      </c>
-      <c r="C19" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F19" s="42" t="s">
-        <v>148</v>
+      <c r="B19" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F19" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="36" t="s">
-        <v>178</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="36" t="s">
-        <v>179</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>180</v>
-      </c>
-      <c r="F20" s="41" t="s">
-        <v>148</v>
+      <c r="B20" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="F20" s="50" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F21" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F22" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D23" s="28" t="s">
         <v>182</v>
       </c>
-      <c r="C21" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D21" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F21" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="36" t="s">
-        <v>183</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="36" t="s">
+      <c r="E23" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F23" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="E22" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="s">
-        <v>184</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>146</v>
-      </c>
-      <c r="D23" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="F23" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
-        <v>209</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="E24" s="36" t="s">
-        <v>189</v>
-      </c>
-      <c r="F24" s="43" t="s">
-        <v>148</v>
+      <c r="F24" s="52" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C25" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F25" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F26" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D27" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F25" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="36" t="s">
-        <v>192</v>
-      </c>
-      <c r="C26" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="F26" s="43" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="40" t="s">
-        <v>193</v>
-      </c>
-      <c r="C27" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>194</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F27" s="42" t="s">
-        <v>148</v>
+      <c r="E27" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D28" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" s="33" t="s">
         <v>195</v>
       </c>
-      <c r="E28" s="46" t="s">
+      <c r="F29" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C30" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="F30" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="F28" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="C29" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="36" t="s">
-        <v>197</v>
-      </c>
-      <c r="E29" s="47" t="s">
-        <v>199</v>
-      </c>
-      <c r="F29" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="40" t="s">
+      <c r="C31" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="27" t="s">
         <v>201</v>
       </c>
-      <c r="C30" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D30" s="45" t="s">
+      <c r="E31" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F31" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="E30" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="F30" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="36" t="s">
-        <v>200</v>
-      </c>
-      <c r="C31" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="36" t="s">
-        <v>205</v>
-      </c>
-      <c r="E31" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="F31" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="40" t="s">
-        <v>206</v>
-      </c>
-      <c r="C32" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D32" s="40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F32" s="42" t="s">
-        <v>148</v>
+      <c r="C32" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="E33" s="46" t="s">
-        <v>208</v>
-      </c>
-      <c r="F33" s="39" t="s">
-        <v>148</v>
+        <v>203</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F33" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="F34" s="39" t="s">
-        <v>148</v>
+        <v>213</v>
+      </c>
+      <c r="F34" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="E35" s="15" t="s">
-        <v>221</v>
-      </c>
-      <c r="F35" s="39" t="s">
-        <v>148</v>
+        <v>217</v>
+      </c>
+      <c r="F35" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="F36" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B37" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="15" t="s">
+      <c r="C37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="F37" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B38" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="F36" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="C37" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="36" t="s">
+      <c r="C38" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D38" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="E37" s="36" t="s">
-        <v>227</v>
-      </c>
-      <c r="F37" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="40" t="s">
-        <v>229</v>
-      </c>
-      <c r="C38" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D38" s="40" t="s">
-        <v>230</v>
-      </c>
-      <c r="E38" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="F38" s="42" t="s">
-        <v>148</v>
+      <c r="E38" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F38" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="C39" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>234</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="F39" s="39" t="s">
-        <v>148</v>
+      <c r="F39" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="31"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2271,286 +2534,1404 @@
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>236</v>
-      </c>
-      <c r="E41" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="F41" s="39" t="s">
-        <v>148</v>
+        <v>232</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="F41" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>239</v>
-      </c>
-      <c r="E42" s="46" t="s">
-        <v>241</v>
-      </c>
-      <c r="F42" s="39" t="s">
-        <v>148</v>
+        <v>235</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="F42" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="39" t="s">
-        <v>148</v>
+        <v>238</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F43" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C44" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F44" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B45" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="15" t="s">
+      <c r="C45" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F45" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B46" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="E44" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="F44" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="C45" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="36" t="s">
+      <c r="C46" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="E45" s="36" t="s">
-        <v>247</v>
-      </c>
-      <c r="F45" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D46" s="40" t="s">
-        <v>176</v>
-      </c>
-      <c r="E46" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F46" s="42" t="s">
-        <v>148</v>
+      <c r="F46" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>251</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>253</v>
-      </c>
-      <c r="F47" s="39" t="s">
-        <v>148</v>
+        <v>247</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F47" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C48" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>256</v>
-      </c>
-      <c r="F48" s="39" t="s">
-        <v>148</v>
+        <v>250</v>
+      </c>
+      <c r="E48" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="F48" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C49" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E49" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="F49" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="15" t="s">
+      <c r="C50" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="27" t="s">
         <v>258</v>
       </c>
-      <c r="E49" s="46" t="s">
+      <c r="E50" s="33" t="s">
         <v>259</v>
       </c>
-      <c r="F49" s="39" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="36" t="s">
+      <c r="F50" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="30" t="s">
         <v>261</v>
       </c>
-      <c r="C50" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="36" t="s">
+      <c r="C51" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D51" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="E51" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F51" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="E50" s="47" t="s">
+      <c r="C52" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F52" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="F50" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="40" t="s">
-        <v>265</v>
-      </c>
-      <c r="C51" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D51" s="40" t="s">
-        <v>264</v>
-      </c>
-      <c r="E51" s="40" t="s">
-        <v>177</v>
-      </c>
-      <c r="F51" s="42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="36" t="s">
+      <c r="C53" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D53" s="30" t="s">
         <v>266</v>
       </c>
-      <c r="C52" s="36" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="36" t="s">
-        <v>271</v>
-      </c>
-      <c r="E52" s="36" t="s">
-        <v>154</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="40" t="s">
-        <v>267</v>
-      </c>
-      <c r="C53" s="40" t="s">
-        <v>146</v>
-      </c>
-      <c r="D53" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="E53" s="40" t="s">
-        <v>156</v>
-      </c>
-      <c r="F53" s="42" t="s">
-        <v>148</v>
+      <c r="E53" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F53" s="51" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C54" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>269</v>
-      </c>
-      <c r="F54" s="39" t="s">
-        <v>148</v>
+        <v>265</v>
+      </c>
+      <c r="F54" s="53" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="48"/>
+      <c r="F55" s="54"/>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="48"/>
+      <c r="F56" s="54"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="34" t="s">
+    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="C58" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="D58" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E58" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="E59" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="F59" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="C60" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="E60" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="F60" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="26"/>
+      <c r="D61" s="43"/>
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="15" t="s">
+        <v>277</v>
+      </c>
+      <c r="C62" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="C58" s="34" t="s">
-        <v>273</v>
-      </c>
-      <c r="D58" s="34" t="s">
+      <c r="E62" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="F62" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="C63" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D63" t="s">
+        <v>284</v>
+      </c>
+      <c r="E63" t="s">
+        <v>283</v>
+      </c>
+      <c r="F63" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="15" t="s">
+        <v>285</v>
+      </c>
+      <c r="C64" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
+        <v>286</v>
+      </c>
+      <c r="E64" t="s">
+        <v>287</v>
+      </c>
+      <c r="F64" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C65" s="26"/>
+      <c r="D65" s="43"/>
+      <c r="E65" s="26"/>
+      <c r="F65" s="26"/>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="27" t="s">
+        <v>294</v>
+      </c>
+      <c r="C66" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="46" t="s">
+        <v>299</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F66" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="30" t="s">
+        <v>295</v>
+      </c>
+      <c r="C67" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D67" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>145</v>
+      </c>
+      <c r="F67" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="27" t="s">
+        <v>296</v>
+      </c>
+      <c r="C68" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="E68" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="F68" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="28" t="s">
+        <v>297</v>
+      </c>
+      <c r="C69" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D69" s="28" t="s">
+        <v>291</v>
+      </c>
+      <c r="E69" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F69" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="28" t="s">
+        <v>298</v>
+      </c>
+      <c r="C70" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D70" s="28" t="s">
+        <v>293</v>
+      </c>
+      <c r="E70" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F70" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="27" t="s">
+        <v>289</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="E71" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F71" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="28" t="s">
+        <v>290</v>
+      </c>
+      <c r="C72" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D72" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E72" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F72" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="28" t="s">
+        <v>292</v>
+      </c>
+      <c r="C73" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D73" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F73" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="27" t="s">
+        <v>300</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="F74" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="C75" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E75" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F75" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="27" t="s">
+        <v>302</v>
+      </c>
+      <c r="C76" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="E76" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="F76" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="E77" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="F77" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C78" s="25"/>
+      <c r="D78" s="29"/>
+      <c r="E78" s="25"/>
+      <c r="F78" s="26"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E79" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="F79" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D80" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E80" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F80" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="C81" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="27" t="s">
+        <v>175</v>
+      </c>
+      <c r="E81" s="27" t="s">
+        <v>176</v>
+      </c>
+      <c r="F81" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="28" t="s">
+        <v>178</v>
+      </c>
+      <c r="C82" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D82" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="E82" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F82" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="27" t="s">
+        <v>179</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>181</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F83" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="C84" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D84" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E84" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F84" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="F85" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C86" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="E86" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="F86" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="27" t="s">
+        <v>188</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="E87" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F87" s="52" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B88" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="C88" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D88" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F88" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B89" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="E89" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="F89" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B90" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="E90" s="33" t="s">
+        <v>195</v>
+      </c>
+      <c r="F90" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B91" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="C91" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D91" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="E91" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="F91" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B92" s="27" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F92" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B93" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="C93" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D93" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="E93" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F93" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B94" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C94" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E94" s="32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F94" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="F95" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="15" t="s">
+        <v>218</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="E96" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F96" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B97" s="15" t="s">
+        <v>220</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>221</v>
+      </c>
+      <c r="F97" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E98" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="F98" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="C99" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F99" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B100" s="15" t="s">
+        <v>227</v>
+      </c>
+      <c r="C100" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="E100" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="F100" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B101" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C101" s="35"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="36"/>
+      <c r="F101" s="37"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B102" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="E102" s="32" t="s">
+        <v>233</v>
+      </c>
+      <c r="F102" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B103" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="E103" s="32" t="s">
+        <v>237</v>
+      </c>
+      <c r="F103" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B104" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="E104" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F104" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B105" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C105" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>242</v>
+      </c>
+      <c r="F105" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B106" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="C106" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>169</v>
+      </c>
+      <c r="E106" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="F106" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="30" t="s">
+        <v>245</v>
+      </c>
+      <c r="C107" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D107" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="E107" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F107" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B108" s="15" t="s">
+        <v>248</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>249</v>
+      </c>
+      <c r="F108" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B109" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>252</v>
+      </c>
+      <c r="F109" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B110" s="15" t="s">
+        <v>253</v>
+      </c>
+      <c r="C110" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>255</v>
+      </c>
+      <c r="F110" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="C111" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="E111" s="33" t="s">
+        <v>259</v>
+      </c>
+      <c r="F111" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="C112" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D112" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="E112" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F112" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="27" t="s">
+        <v>262</v>
+      </c>
+      <c r="C113" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E113" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F113" s="50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="C114" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>152</v>
+      </c>
+      <c r="F114" s="51" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>256</v>
+      </c>
+      <c r="E115" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="F115" s="53" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B117" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B118" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="C118" s="26" t="s">
+        <v>269</v>
+      </c>
+      <c r="D118" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E58" s="34" t="s">
+      <c r="E118" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="34" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="34" t="s">
-        <v>43</v>
-      </c>
-      <c r="C59" s="34"/>
-      <c r="D59" s="34"/>
-      <c r="E59" s="34"/>
-      <c r="F59" s="44"/>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F60" s="48"/>
+      <c r="F118" s="26" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B119" s="27" t="s">
+        <v>306</v>
+      </c>
+      <c r="C119" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="27" t="s">
+        <v>304</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>309</v>
+      </c>
+      <c r="F119" s="56" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B120" s="28" t="s">
+        <v>307</v>
+      </c>
+      <c r="C120" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D120" s="28" t="s">
+        <v>312</v>
+      </c>
+      <c r="E120" s="55" t="s">
+        <v>310</v>
+      </c>
+      <c r="F120" s="58" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B121" s="30" t="s">
+        <v>311</v>
+      </c>
+      <c r="C121" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D121" s="30" t="s">
+        <v>308</v>
+      </c>
+      <c r="E121" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F121" s="57" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="15" t="s">
+        <v>314</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="15" t="s">
+        <v>315</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="F122" s="48" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="27" t="s">
+        <v>319</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="27" t="s">
+        <v>317</v>
+      </c>
+      <c r="E123" s="33" t="s">
+        <v>318</v>
+      </c>
+      <c r="F123" s="56" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B124" s="28" t="s">
+        <v>320</v>
+      </c>
+      <c r="C124" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="D124" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="E124" s="55" t="s">
+        <v>310</v>
+      </c>
+      <c r="F124" s="58" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="C125" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D125" s="30" t="s">
+        <v>323</v>
+      </c>
+      <c r="E125" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F125" s="57" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B126" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="C126" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="E126" s="33" t="s">
+        <v>325</v>
+      </c>
+      <c r="F126" s="56" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="30" t="s">
+        <v>326</v>
+      </c>
+      <c r="C127" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D127" s="30" t="s">
+        <v>327</v>
+      </c>
+      <c r="E127" s="31" t="s">
+        <v>310</v>
+      </c>
+      <c r="F127" s="57" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="E128" s="32" t="s">
+        <v>331</v>
+      </c>
+      <c r="F128" s="53" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="C40:F40"/>
+    <mergeCell ref="C101:F101"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2559,10 +3940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K98"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A64" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2578,10 +3959,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="41"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -2611,10 +3992,10 @@
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="31"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -2646,7 +4027,7 @@
         <v>24</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>7</v>
@@ -2684,7 +4065,7 @@
         <v>26</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>7</v>
@@ -2698,7 +4079,7 @@
     </row>
     <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>18</v>
@@ -2716,10 +4097,10 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>12</v>
@@ -2733,10 +4114,10 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -2752,10 +4133,10 @@
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
-      <c r="F13" s="31"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -2784,7 +4165,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>7</v>
@@ -2801,7 +4182,7 @@
         <v>29</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>7</v>
@@ -2818,7 +4199,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D17" s="13" t="s">
         <v>7</v>
@@ -2835,7 +4216,7 @@
         <v>31</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>7</v>
@@ -2853,7 +4234,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>7</v>
@@ -2868,10 +4249,10 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>7</v>
@@ -2886,10 +4267,10 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>12</v>
@@ -2904,10 +4285,10 @@
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>12</v>
@@ -2922,10 +4303,10 @@
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>12</v>
@@ -2940,10 +4321,10 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>7</v>
@@ -2958,10 +4339,10 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D25" s="18" t="s">
         <v>7</v>
@@ -2976,7 +4357,7 @@
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>22</v>
@@ -2994,10 +4375,10 @@
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>7</v>
@@ -3012,10 +4393,10 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>7</v>
@@ -3032,10 +4413,10 @@
       <c r="B29" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="30"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="36"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="37"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -3047,7 +4428,7 @@
         <v>33</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>7</v>
@@ -3065,7 +4446,7 @@
         <v>34</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>7</v>
@@ -3083,7 +4464,7 @@
         <v>35</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>7</v>
@@ -3134,10 +4515,10 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>7</v>
@@ -3152,10 +4533,10 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D36" s="18" t="s">
         <v>7</v>
@@ -3170,10 +4551,10 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="18" t="s">
         <v>7</v>
@@ -3188,10 +4569,10 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D38" s="18" t="s">
         <v>7</v>
@@ -3206,10 +4587,10 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C39" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D39" s="18" t="s">
         <v>7</v>
@@ -3224,10 +4605,10 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="20" t="s">
         <v>7</v>
@@ -3303,10 +4684,10 @@
       <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="27"/>
+      <c r="C45" s="35"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="38"/>
+      <c r="F45" s="39"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -3335,10 +4716,10 @@
         <v>45</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>93</v>
+        <v>281</v>
       </c>
       <c r="D47" s="18" t="s">
-        <v>12</v>
+        <v>282</v>
       </c>
       <c r="E47" s="13" t="s">
         <v>8</v>
@@ -3353,63 +4734,67 @@
         <v>46</v>
       </c>
       <c r="C48" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D48" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E48" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="9" t="s">
+      <c r="E48" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G48" s="13"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="C49" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G49" s="13"/>
+      <c r="B49" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="35"/>
+      <c r="D49" s="36"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="1"/>
+      <c r="K49" s="1"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="31"/>
-      <c r="G50" s="1"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C51" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F51" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G51" s="21"/>
@@ -3417,34 +4802,29 @@
       <c r="J51" s="21"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
+    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="E52" s="13" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G52" s="21"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="21"/>
-      <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="15" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>7</v>
@@ -3456,15 +4836,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="D54" s="13" t="s">
+        <v>12</v>
       </c>
       <c r="E54" s="13" t="s">
         <v>8</v>
@@ -3472,13 +4852,14 @@
       <c r="F54" s="9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="55" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>18</v>
+        <v>53</v>
       </c>
       <c r="D55" s="13" t="s">
         <v>12</v>
@@ -3489,14 +4870,13 @@
       <c r="F55" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G55" s="13"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C56" s="15" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D56" s="13" t="s">
         <v>12</v>
@@ -3509,42 +4889,42 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="C57" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D57" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E57" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="B57" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57" s="35"/>
+      <c r="D57" s="36"/>
+      <c r="E57" s="36"/>
+      <c r="F57" s="37"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
-      <c r="F58" s="31"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
+      <c r="B58" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="C58" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E58" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>20</v>
+        <v>61</v>
       </c>
       <c r="D59" s="13" t="s">
         <v>7</v>
@@ -3558,7 +4938,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>62</v>
@@ -3575,7 +4955,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C61" s="15" t="s">
         <v>63</v>
@@ -3592,12 +4972,12 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C62" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="C62" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="D62" s="13" t="s">
+      <c r="D62" s="8" t="s">
         <v>7</v>
       </c>
       <c r="E62" s="13" t="s">
@@ -3606,10 +4986,11 @@
       <c r="F62" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="G62" s="13"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>65</v>
@@ -3627,7 +5008,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>66</v>
@@ -3645,13 +5026,13 @@
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C65" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D65" s="8" t="s">
-        <v>7</v>
+        <v>117</v>
+      </c>
+      <c r="C65" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>8</v>
@@ -3663,7 +5044,7 @@
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C66" s="15" t="s">
         <v>70</v>
@@ -3681,7 +5062,7 @@
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C67" s="15" t="s">
         <v>71</v>
@@ -3699,13 +5080,13 @@
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C68" s="15" t="s">
-        <v>72</v>
+        <v>120</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>67</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E68" s="13" t="s">
         <v>8</v>
@@ -3717,7 +5098,7 @@
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>68</v>
@@ -3735,13 +5116,13 @@
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C70" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D70" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E70" s="13" t="s">
         <v>8</v>
@@ -3753,13 +5134,13 @@
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C71" s="17" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="E71" s="13" t="s">
         <v>8</v>
@@ -3771,12 +5152,12 @@
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="D72" s="8" t="s">
+      <c r="D72" s="10" t="s">
         <v>7</v>
       </c>
       <c r="E72" s="13" t="s">
@@ -3788,40 +5169,40 @@
       <c r="G72" s="13"/>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C73" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E73" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G73" s="13"/>
+      <c r="B73" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C73" s="35"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="37"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C74" s="25"/>
-      <c r="D74" s="30"/>
-      <c r="E74" s="30"/>
-      <c r="F74" s="31"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
+      <c r="B74" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D74" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G74" s="13"/>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C75" s="15" t="s">
         <v>84</v>
@@ -3839,10 +5220,10 @@
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C76" s="15" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="D76" s="13" t="s">
         <v>7</v>
@@ -3857,13 +5238,13 @@
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D77" s="13" t="s">
-        <v>7</v>
+        <v>128</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D77" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="E77" s="13" t="s">
         <v>8</v>
@@ -3875,13 +5256,13 @@
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="C78" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D78" s="18" t="s">
-        <v>12</v>
+        <v>129</v>
+      </c>
+      <c r="C78" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D78" s="13" t="s">
+        <v>7</v>
       </c>
       <c r="E78" s="13" t="s">
         <v>8</v>
@@ -3893,12 +5274,12 @@
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="C79" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D79" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79" s="18" t="s">
         <v>7</v>
       </c>
       <c r="E79" s="13" t="s">
@@ -3911,7 +5292,7 @@
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>86</v>
@@ -3925,11 +5306,11 @@
       <c r="F80" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G80" s="13"/>
+      <c r="G80" s="18"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>87</v>
@@ -3940,17 +5321,17 @@
       <c r="E81" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="F81" s="9" t="s">
+      <c r="F81" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G81" s="18"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B82" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D82" s="18" t="s">
         <v>7</v>
@@ -3965,12 +5346,12 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="D83" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="C83" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D83" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E83" s="13" t="s">
@@ -3983,73 +5364,78 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B84" s="15" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="C84" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="D84" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E84" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="D84" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F84" s="11" t="s">
         <v>9</v>
       </c>
       <c r="G84" s="18"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B85" s="15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C85" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="D85" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="G85" s="18"/>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-      <c r="E86" s="2"/>
-      <c r="F86" s="2"/>
+      <c r="B86" s="16" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G87" s="1"/>
+      <c r="H87" s="1"/>
+      <c r="I87" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J87" s="1"/>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="2"/>
+      <c r="B88" s="15" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B88" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C88" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E88" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G88" s="1"/>
+      <c r="C88" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D88" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F88" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G88" s="22"/>
       <c r="H88" s="1"/>
-      <c r="I88" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I88" s="22"/>
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
@@ -4059,15 +5445,15 @@
         <v>52</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>97</v>
-      </c>
-      <c r="D89" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E89" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F89" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F89" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G89" s="22"/>
@@ -4079,10 +5465,10 @@
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="15" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D90" s="8" t="s">
         <v>7</v>
@@ -4102,10 +5488,10 @@
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="15" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C91" s="17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>7</v>
@@ -4122,84 +5508,61 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
+    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D92" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F92" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D92" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F92" s="12" t="s">
         <v>9</v>
       </c>
       <c r="G92" s="22"/>
-      <c r="H92" s="1"/>
-      <c r="I92" s="22"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-    </row>
-    <row r="93" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="C93" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D93" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E93" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F93" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G93" s="22"/>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="13"/>
-      <c r="E94" s="13"/>
-      <c r="F94" s="2"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="2"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B95" s="24" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="24" t="s">
-        <v>4</v>
-      </c>
+      <c r="B96" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" s="40"/>
+      <c r="D96" s="40"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B97" s="28" t="s">
-        <v>141</v>
-      </c>
-      <c r="C97" s="28"/>
-      <c r="D97" s="28"/>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B98" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C98" s="21"/>
-      <c r="D98" s="21"/>
+      <c r="B97" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="C97" s="21"/>
+      <c r="D97" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="C45:F45"/>
-    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B96:D96"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C5:F5"/>
     <mergeCell ref="C13:F13"/>
     <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C50:F50"/>
-    <mergeCell ref="C58:F58"/>
-    <mergeCell ref="C74:F74"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="C57:F57"/>
+    <mergeCell ref="C73:F73"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update cahier des tests
</commit_message>
<xml_diff>
--- a/annexes/Cahier_de_test.xlsx
+++ b/annexes/Cahier_de_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\rosetta\annexes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christophe\Documents\IUT\projet\Rosetta\git\rosetta\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD3108A-12CC-44C2-B5F2-4C2648A018D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2B165C-C9AF-4B85-8790-DE4D0E5001F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="2" r:id="rId1"/>
@@ -508,9 +508,6 @@
     <t>Rechercher un client qui n'existe pas</t>
   </si>
   <si>
-    <t>Non tester</t>
-  </si>
-  <si>
     <t>Affichage d'aucun client ou d'un message le précisant</t>
   </si>
   <si>
@@ -1116,6 +1113,9 @@
   </si>
   <si>
     <t>Synchronisation des donnée entre la tablette et le site web</t>
+  </si>
+  <si>
+    <t>Non testé</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1491,30 +1491,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1540,15 +1516,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1560,6 +1527,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1885,38 +1876,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D569B6-B3CB-4EA1-907F-9E75FD9F6494}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="E130" sqref="E130"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.140625" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="34" t="s">
+    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>268</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>269</v>
       </c>
       <c r="D4" s="26" t="s">
         <v>5</v>
@@ -1925,20 +1916,20 @@
         <v>10</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="25"/>
       <c r="D5" s="29"/>
       <c r="E5" s="25"/>
-      <c r="F5" s="49"/>
+      <c r="F5" s="41"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
         <v>139</v>
       </c>
@@ -1949,14 +1940,14 @@
         <v>141</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="F6" s="50" t="s">
-        <v>144</v>
+        <v>148</v>
+      </c>
+      <c r="F6" s="42" t="s">
+        <v>331</v>
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B7" s="30" t="s">
         <v>140</v>
       </c>
@@ -1967,170 +1958,170 @@
         <v>143</v>
       </c>
       <c r="E7" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B8" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="F7" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="27" t="s">
+      <c r="C8" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F8" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="28" t="s">
         <v>146</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F8" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
-        <v>147</v>
       </c>
       <c r="C9" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D9" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="F9" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="30" t="s">
         <v>152</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
-        <v>153</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D10" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E10" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E10" s="30" t="s">
+      <c r="F10" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="F10" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="27" t="s">
+      <c r="C11" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="27" t="s">
         <v>156</v>
       </c>
-      <c r="C11" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="E11" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="E11" s="27" t="s">
+      <c r="F11" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="30" t="s">
         <v>158</v>
-      </c>
-      <c r="F11" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="30" t="s">
-        <v>159</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="F12" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="F12" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="27" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F13" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+      <c r="F13" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="27" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="E14" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F14" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="F15" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
       <c r="B16" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="E16" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="E16" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F16" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
       <c r="B17" s="26" t="s">
         <v>19</v>
@@ -2140,653 +2131,653 @@
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
       <c r="B18" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="C18" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="27" t="s">
+      <c r="E18" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E18" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="30" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D19" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="E19" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F19" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
       <c r="B20" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="C20" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="27" t="s">
+      <c r="E20" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="E20" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F20" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F20" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
       <c r="B21" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F21" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F21" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F22" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="C22" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E22" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F22" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="28" t="s">
-        <v>180</v>
       </c>
       <c r="C23" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E23" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F23" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F24" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E24" s="27" t="s">
+      <c r="C25" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="F24" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D25" s="30" t="s">
+      <c r="E25" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F25" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E25" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F25" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="27" t="s">
+      <c r="E26" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F26" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="30" t="s">
         <v>188</v>
-      </c>
-      <c r="C26" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F26" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
-        <v>189</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D27" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F27" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E27" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F27" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="15" t="s">
+      <c r="E28" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="F28" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="F28" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
+      <c r="E29" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C29" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="F29" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F29" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B30" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D30" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E30" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="E30" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="F30" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F30" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B31" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D31" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E31" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F31" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B32" s="30" t="s">
         <v>201</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F31" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="30" t="s">
-        <v>202</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D32" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E32" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="E32" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F32" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F32" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D33" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E33" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="E33" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="F33" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F33" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F34" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B35" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C34" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="15" t="s">
+      <c r="E35" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="F35" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B36" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D36" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="F35" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="15" t="s">
+      <c r="E36" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C36" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E36" s="15" t="s">
+      <c r="F36" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D37" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="F36" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="27" t="s">
+      <c r="E37" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="30" t="s">
         <v>224</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="E37" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="F37" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="30" t="s">
-        <v>225</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D38" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="E38" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F38" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="15" t="s">
-        <v>227</v>
-      </c>
       <c r="C39" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D39" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E39" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="E39" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F39" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F39" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B40" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="37"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="51"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B41" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C41" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="F41" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C42" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="C41" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="E41" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="F41" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
+      <c r="E42" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C42" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D42" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E42" s="32" t="s">
+      <c r="F42" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="F42" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="E43" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F43" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C43" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E43" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="F43" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+      <c r="C44" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C44" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="15" t="s">
+      <c r="E44" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="E44" s="32" t="s">
+      <c r="F44" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E45" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="F44" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="27" t="s">
+      <c r="F45" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="30" t="s">
         <v>244</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D45" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="F45" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="30" t="s">
-        <v>245</v>
       </c>
       <c r="C46" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D46" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="E46" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F46" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="F46" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B47" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C47" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E47" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="C47" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="E47" s="32" t="s">
+      <c r="F47" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C48" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D48" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="F47" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="15" t="s">
+      <c r="E48" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C48" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="E48" s="32" t="s">
+      <c r="F48" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="F48" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="15" t="s">
+      <c r="C49" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C49" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D49" s="15" t="s">
+      <c r="E49" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="E49" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="F49" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B50" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C50" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="C50" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D50" s="27" t="s">
+      <c r="E50" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="E50" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="F50" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F50" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B51" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C51" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E51" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F51" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F51" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B52" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F52" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53" s="30" t="s">
         <v>262</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="E52" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F52" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="30" t="s">
-        <v>263</v>
       </c>
       <c r="C53" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D53" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F53" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F53" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B54" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C54" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F54" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F55" s="54"/>
-    </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F56" s="54"/>
-    </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F54" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="43"/>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="43"/>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C58" s="26" t="s">
         <v>268</v>
-      </c>
-      <c r="C58" s="26" t="s">
-        <v>269</v>
       </c>
       <c r="D58" s="26" t="s">
         <v>5</v>
@@ -2795,317 +2786,317 @@
         <v>10</v>
       </c>
       <c r="F58" s="26" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="C59" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59" s="34" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="42" t="s">
+      <c r="E59" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="F59" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60" s="34" t="s">
         <v>273</v>
-      </c>
-      <c r="C59" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D59" s="42" t="s">
-        <v>271</v>
-      </c>
-      <c r="E59" s="42" t="s">
-        <v>278</v>
-      </c>
-      <c r="F59" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="42" t="s">
-        <v>274</v>
       </c>
       <c r="C60" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="D60" s="42" t="s">
+      <c r="D60" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="E60" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="E60" s="42" t="s">
-        <v>276</v>
-      </c>
-      <c r="F60" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F60" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B61" s="26" t="s">
         <v>43</v>
       </c>
       <c r="C61" s="26"/>
-      <c r="D61" s="43"/>
+      <c r="D61" s="35"/>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B62" s="15" t="s">
-        <v>277</v>
-      </c>
-      <c r="C62" s="45" t="s">
+        <v>276</v>
+      </c>
+      <c r="C62" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E62" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="F62" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63" s="15" t="s">
         <v>279</v>
       </c>
-      <c r="F62" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="15" t="s">
-        <v>280</v>
-      </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="37" t="s">
         <v>11</v>
       </c>
       <c r="D63" t="s">
+        <v>283</v>
+      </c>
+      <c r="E63" t="s">
+        <v>282</v>
+      </c>
+      <c r="F63" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="E63" t="s">
-        <v>283</v>
-      </c>
-      <c r="F63" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="15" t="s">
+      <c r="C64" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D64" t="s">
         <v>285</v>
       </c>
-      <c r="C64" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>286</v>
       </c>
-      <c r="E64" t="s">
-        <v>287</v>
-      </c>
-      <c r="F64" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="26" t="s">
         <v>15</v>
       </c>
       <c r="C65" s="26"/>
-      <c r="D65" s="43"/>
+      <c r="D65" s="35"/>
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B66" s="27" t="s">
+        <v>293</v>
+      </c>
+      <c r="C66" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" s="38" t="s">
+        <v>298</v>
+      </c>
+      <c r="E66" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F66" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67" s="30" t="s">
         <v>294</v>
-      </c>
-      <c r="C66" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D66" s="46" t="s">
-        <v>299</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="30" t="s">
-        <v>295</v>
       </c>
       <c r="C67" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="D67" s="47" t="s">
+      <c r="D67" s="39" t="s">
         <v>143</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="F67" s="52" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B68" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="C68" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D68" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="E68" s="27" t="s">
+        <v>287</v>
+      </c>
+      <c r="F68" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69" s="28" t="s">
         <v>296</v>
-      </c>
-      <c r="C68" s="44" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="27" t="s">
-        <v>157</v>
-      </c>
-      <c r="E68" s="27" t="s">
-        <v>288</v>
-      </c>
-      <c r="F68" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="28" t="s">
-        <v>297</v>
       </c>
       <c r="C69" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D69" s="28" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E69" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F69" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F69" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B70" s="28" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C70" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D70" s="28" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="F70" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="F70" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B71" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="C71" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D71" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="E71" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F71" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72" s="28" t="s">
         <v>289</v>
-      </c>
-      <c r="C71" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D71" s="27" t="s">
-        <v>148</v>
-      </c>
-      <c r="E71" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F71" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="28" t="s">
-        <v>290</v>
       </c>
       <c r="C72" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D72" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="E72" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="E72" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F72" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F72" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B73" s="28" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C73" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D73" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="E73" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="E73" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="F73" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F73" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="27" t="s">
+        <v>299</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E74" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="F74" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75" s="27" t="s">
         <v>300</v>
       </c>
-      <c r="C74" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D74" s="15" t="s">
+      <c r="C75" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="E74" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="F74" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="27" t="s">
+      <c r="E75" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F75" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76" s="27" t="s">
         <v>301</v>
       </c>
-      <c r="C75" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="E75" s="15" t="s">
+      <c r="C76" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="F75" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="27" t="s">
+      <c r="E76" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="F76" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77" s="27" t="s">
         <v>302</v>
       </c>
-      <c r="C76" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="E76" s="15" t="s">
+      <c r="C77" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="F76" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="27" t="s">
-        <v>303</v>
-      </c>
-      <c r="C77" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="15" t="s">
+      <c r="E77" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="E77" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="F77" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F77" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B78" s="26" t="s">
         <v>19</v>
       </c>
@@ -3114,638 +3105,638 @@
       <c r="E78" s="25"/>
       <c r="F78" s="26"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B79" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C79" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="27" t="s">
         <v>168</v>
       </c>
-      <c r="C79" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D79" s="27" t="s">
+      <c r="E79" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="E79" s="27" t="s">
+      <c r="F79" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80" s="30" t="s">
         <v>170</v>
-      </c>
-      <c r="F79" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="30" t="s">
-        <v>171</v>
       </c>
       <c r="C80" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D80" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E80" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="E80" s="30" t="s">
+      <c r="F80" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="F80" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="27" t="s">
+      <c r="C81" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="C81" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D81" s="27" t="s">
+      <c r="E81" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="E81" s="27" t="s">
-        <v>176</v>
-      </c>
-      <c r="F81" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F81" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B82" s="28" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C82" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F82" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F82" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B83" s="27" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="E83" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F83" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B84" s="28" t="s">
         <v>179</v>
-      </c>
-      <c r="C83" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" s="27" t="s">
-        <v>181</v>
-      </c>
-      <c r="E83" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F83" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="28" t="s">
-        <v>180</v>
       </c>
       <c r="C84" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E84" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F84" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F84" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B85" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C85" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>183</v>
+      </c>
+      <c r="E85" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="F85" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="C85" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="E85" s="27" t="s">
+      <c r="C86" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="F85" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="15" t="s">
-        <v>206</v>
-      </c>
-      <c r="C86" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D86" s="30" t="s">
+      <c r="E86" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F86" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87" s="27" t="s">
+        <v>187</v>
+      </c>
+      <c r="C87" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="E86" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="F86" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="27" t="s">
+      <c r="E87" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F87" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88" s="30" t="s">
         <v>188</v>
-      </c>
-      <c r="C87" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="E87" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F87" s="52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="30" t="s">
-        <v>189</v>
       </c>
       <c r="C88" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D88" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="E88" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F88" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="C89" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="E88" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F88" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="15" t="s">
-        <v>207</v>
-      </c>
-      <c r="C89" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D89" s="15" t="s">
+      <c r="E89" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="E89" s="32" t="s">
+      <c r="F89" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="C90" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="27" t="s">
         <v>192</v>
       </c>
-      <c r="F89" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="27" t="s">
+      <c r="E90" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C90" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D90" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="E90" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="F90" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F90" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B91" s="30" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C91" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D91" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="E91" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="E91" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="F91" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F91" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B92" s="27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>11</v>
       </c>
       <c r="D92" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E92" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F92" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B93" s="30" t="s">
         <v>201</v>
-      </c>
-      <c r="E92" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F92" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="30" t="s">
-        <v>202</v>
       </c>
       <c r="C93" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D93" s="30" t="s">
+        <v>150</v>
+      </c>
+      <c r="E93" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="E93" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F93" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F93" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B94" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D94" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="E94" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="E94" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="F94" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B95" s="15" t="s">
+        <v>214</v>
+      </c>
+      <c r="C95" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="E95" s="15" t="s">
+        <v>212</v>
+      </c>
+      <c r="F95" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B96" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="C96" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C95" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>214</v>
-      </c>
-      <c r="E95" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="F95" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="15" t="s">
+      <c r="E96" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="F96" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B97" s="15" t="s">
+        <v>219</v>
+      </c>
+      <c r="C97" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C96" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="E96" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="F96" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="15" t="s">
+      <c r="E97" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="C97" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="E97" s="15" t="s">
+      <c r="F97" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B98" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="F97" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="27" t="s">
+      <c r="E98" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F98" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B99" s="30" t="s">
         <v>224</v>
-      </c>
-      <c r="C98" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D98" s="27" t="s">
-        <v>222</v>
-      </c>
-      <c r="E98" s="27" t="s">
-        <v>223</v>
-      </c>
-      <c r="F98" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" s="30" t="s">
-        <v>225</v>
       </c>
       <c r="C99" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D99" s="30" t="s">
+        <v>225</v>
+      </c>
+      <c r="E99" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="F99" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="E99" s="28" t="s">
-        <v>152</v>
-      </c>
-      <c r="F99" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="15" t="s">
-        <v>227</v>
-      </c>
       <c r="C100" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D100" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="E100" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="E100" s="15" t="s">
-        <v>231</v>
-      </c>
-      <c r="F100" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F100" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B101" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C101" s="35"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="37"/>
-    </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C101" s="49"/>
+      <c r="D101" s="50"/>
+      <c r="E101" s="50"/>
+      <c r="F101" s="51"/>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B102" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="C102" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E102" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="F102" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B103" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="C103" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="C102" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D102" s="15" t="s">
-        <v>232</v>
-      </c>
-      <c r="E102" s="32" t="s">
-        <v>233</v>
-      </c>
-      <c r="F102" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B103" s="15" t="s">
+      <c r="E103" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="C103" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D103" s="15" t="s">
-        <v>235</v>
-      </c>
-      <c r="E103" s="32" t="s">
+      <c r="F103" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B104" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="F103" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B104" s="15" t="s">
+      <c r="E104" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="F104" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B105" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C104" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D104" s="15" t="s">
-        <v>238</v>
-      </c>
-      <c r="E104" s="32" t="s">
-        <v>165</v>
-      </c>
-      <c r="F104" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B105" s="15" t="s">
+      <c r="C105" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C105" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D105" s="15" t="s">
+      <c r="E105" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="E105" s="32" t="s">
+      <c r="F105" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B106" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="C106" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="E106" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="F105" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B106" s="27" t="s">
+      <c r="F106" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B107" s="30" t="s">
         <v>244</v>
-      </c>
-      <c r="C106" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" s="27" t="s">
-        <v>169</v>
-      </c>
-      <c r="E106" s="27" t="s">
-        <v>243</v>
-      </c>
-      <c r="F106" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B107" s="30" t="s">
-        <v>245</v>
       </c>
       <c r="C107" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D107" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="E107" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="E107" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F107" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F107" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B108" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="C108" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>246</v>
+      </c>
+      <c r="E108" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="C108" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D108" s="15" t="s">
-        <v>247</v>
-      </c>
-      <c r="E108" s="32" t="s">
+      <c r="F108" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B109" s="15" t="s">
+        <v>250</v>
+      </c>
+      <c r="C109" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="15" t="s">
         <v>249</v>
       </c>
-      <c r="F108" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B109" s="15" t="s">
+      <c r="E109" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="C109" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D109" s="15" t="s">
-        <v>250</v>
-      </c>
-      <c r="E109" s="32" t="s">
+      <c r="F109" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B110" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="F109" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B110" s="15" t="s">
+      <c r="C110" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="C110" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D110" s="15" t="s">
+      <c r="E110" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="E110" s="32" t="s">
-        <v>255</v>
-      </c>
-      <c r="F110" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F110" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B111" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="C111" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="27" t="s">
         <v>257</v>
       </c>
-      <c r="C111" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D111" s="27" t="s">
+      <c r="E111" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="E111" s="33" t="s">
-        <v>259</v>
-      </c>
-      <c r="F111" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F111" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B112" s="30" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C112" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D112" s="30" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="F112" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+      <c r="F112" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B113" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="C113" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="27" t="s">
+        <v>266</v>
+      </c>
+      <c r="E113" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="F113" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B114" s="30" t="s">
         <v>262</v>
-      </c>
-      <c r="C113" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" s="27" t="s">
-        <v>267</v>
-      </c>
-      <c r="E113" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="F113" s="50" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="30" t="s">
-        <v>263</v>
       </c>
       <c r="C114" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D114" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="F114" s="51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="F114" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B115" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="C115" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="15" t="s">
+        <v>255</v>
+      </c>
+      <c r="E115" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C115" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D115" s="15" t="s">
-        <v>256</v>
-      </c>
-      <c r="E115" s="15" t="s">
-        <v>265</v>
-      </c>
-      <c r="F115" s="53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F115" s="42" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B117" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B118" s="26" t="s">
+        <v>267</v>
+      </c>
+      <c r="C118" s="26" t="s">
         <v>268</v>
-      </c>
-      <c r="C118" s="26" t="s">
-        <v>269</v>
       </c>
       <c r="D118" s="26" t="s">
         <v>5</v>
@@ -3754,177 +3745,177 @@
         <v>10</v>
       </c>
       <c r="F118" s="26" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B119" s="27" t="s">
+        <v>305</v>
+      </c>
+      <c r="C119" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="27" t="s">
+        <v>303</v>
+      </c>
+      <c r="E119" s="27" t="s">
+        <v>308</v>
+      </c>
+      <c r="F119" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B120" s="28" t="s">
         <v>306</v>
-      </c>
-      <c r="C119" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D119" s="27" t="s">
-        <v>304</v>
-      </c>
-      <c r="E119" s="27" t="s">
-        <v>309</v>
-      </c>
-      <c r="F119" s="56" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B120" s="28" t="s">
-        <v>307</v>
       </c>
       <c r="C120" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D120" s="28" t="s">
-        <v>312</v>
-      </c>
-      <c r="E120" s="55" t="s">
+        <v>311</v>
+      </c>
+      <c r="E120" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="F120" s="47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B121" s="30" t="s">
         <v>310</v>
-      </c>
-      <c r="F120" s="58" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B121" s="30" t="s">
-        <v>311</v>
       </c>
       <c r="C121" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D121" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E121" s="31" t="s">
-        <v>310</v>
-      </c>
-      <c r="F121" s="57" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="F121" s="46" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B122" s="15" t="s">
+        <v>313</v>
+      </c>
+      <c r="C122" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="C122" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D122" s="15" t="s">
+      <c r="E122" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="E122" s="32" t="s">
+      <c r="F122" s="40" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B123" s="27" t="s">
+        <v>318</v>
+      </c>
+      <c r="C123" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="27" t="s">
         <v>316</v>
       </c>
-      <c r="F122" s="48" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B123" s="27" t="s">
+      <c r="E123" s="33" t="s">
+        <v>317</v>
+      </c>
+      <c r="F123" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B124" s="28" t="s">
         <v>319</v>
-      </c>
-      <c r="C123" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D123" s="27" t="s">
-        <v>317</v>
-      </c>
-      <c r="E123" s="33" t="s">
-        <v>318</v>
-      </c>
-      <c r="F123" s="56" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B124" s="28" t="s">
-        <v>320</v>
       </c>
       <c r="C124" s="28" t="s">
         <v>142</v>
       </c>
       <c r="D124" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="E124" s="55" t="s">
-        <v>310</v>
-      </c>
-      <c r="F124" s="58" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+      <c r="E124" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="F124" s="47" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B125" s="30" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C125" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D125" s="30" t="s">
+        <v>322</v>
+      </c>
+      <c r="E125" s="31" t="s">
+        <v>309</v>
+      </c>
+      <c r="F125" s="46" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B126" s="27" t="s">
         <v>323</v>
       </c>
-      <c r="E125" s="31" t="s">
-        <v>310</v>
-      </c>
-      <c r="F125" s="57" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="27" t="s">
+      <c r="C126" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="E126" s="33" t="s">
         <v>324</v>
       </c>
-      <c r="C126" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="D126" s="27" t="s">
-        <v>328</v>
-      </c>
-      <c r="E126" s="33" t="s">
+      <c r="F126" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B127" s="30" t="s">
         <v>325</v>
-      </c>
-      <c r="F126" s="56" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="30" t="s">
-        <v>326</v>
       </c>
       <c r="C127" s="30" t="s">
         <v>142</v>
       </c>
       <c r="D127" s="30" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E127" s="31" t="s">
-        <v>310</v>
-      </c>
-      <c r="F127" s="57" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+      <c r="F127" s="46" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B128" s="15" t="s">
+        <v>329</v>
+      </c>
+      <c r="C128" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D128" s="15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E128" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="C128" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D128" s="15" t="s">
-        <v>329</v>
-      </c>
-      <c r="E128" s="32" t="s">
-        <v>331</v>
-      </c>
-      <c r="F128" s="53" t="s">
-        <v>144</v>
+      <c r="F128" s="42" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>
@@ -3935,6 +3926,7 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3946,30 +3938,30 @@
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="127.140625" customWidth="1"/>
+    <col min="3" max="3" width="127.109375" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" customWidth="1"/>
-    <col min="10" max="10" width="43.5703125" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.109375" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+    <col min="10" max="10" width="43.5546875" customWidth="1"/>
+    <col min="11" max="11" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B1" s="55" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="41"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="55"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3988,18 +3980,18 @@
       <c r="G4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="37"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="51"/>
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="15" t="s">
         <v>23</v>
@@ -4021,7 +4013,7 @@
       <c r="J6" s="21"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>
       <c r="B7" s="15" t="s">
         <v>24</v>
@@ -4043,7 +4035,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>25</v>
       </c>
@@ -4060,7 +4052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
@@ -4077,7 +4069,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
         <v>58</v>
       </c>
@@ -4095,7 +4087,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
         <v>59</v>
       </c>
@@ -4112,7 +4104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
         <v>60</v>
       </c>
@@ -4129,21 +4121,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="37"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="51"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
@@ -4160,7 +4152,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
@@ -4177,7 +4169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
@@ -4194,7 +4186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>30</v>
       </c>
@@ -4211,7 +4203,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>31</v>
       </c>
@@ -4229,7 +4221,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>32</v>
       </c>
@@ -4247,7 +4239,7 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>74</v>
       </c>
@@ -4265,7 +4257,7 @@
       </c>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="15" t="s">
         <v>75</v>
       </c>
@@ -4283,12 +4275,12 @@
       </c>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>12</v>
@@ -4301,7 +4293,7 @@
       </c>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="15" t="s">
         <v>77</v>
       </c>
@@ -4319,7 +4311,7 @@
       </c>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="15" t="s">
         <v>78</v>
       </c>
@@ -4337,7 +4329,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="15" t="s">
         <v>79</v>
       </c>
@@ -4355,7 +4347,7 @@
       </c>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="15" t="s">
         <v>80</v>
       </c>
@@ -4373,12 +4365,12 @@
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="15" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D27" s="8" t="s">
         <v>7</v>
@@ -4391,12 +4383,12 @@
       </c>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C28" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>7</v>
@@ -4409,21 +4401,21 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="36"/>
-      <c r="E29" s="36"/>
-      <c r="F29" s="37"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="51"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="15" t="s">
         <v>33</v>
       </c>
@@ -4441,7 +4433,7 @@
       </c>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="15" t="s">
         <v>34</v>
       </c>
@@ -4459,7 +4451,7 @@
       </c>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
@@ -4477,7 +4469,7 @@
       </c>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B33" s="15" t="s">
         <v>37</v>
       </c>
@@ -4495,7 +4487,7 @@
       </c>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B34" s="15" t="s">
         <v>38</v>
       </c>
@@ -4513,12 +4505,12 @@
       </c>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B35" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D35" s="18" t="s">
         <v>7</v>
@@ -4531,7 +4523,7 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B36" s="15" t="s">
         <v>95</v>
       </c>
@@ -4549,7 +4541,7 @@
       </c>
       <c r="G36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B37" s="15" t="s">
         <v>96</v>
       </c>
@@ -4567,7 +4559,7 @@
       </c>
       <c r="G37" s="13"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B38" s="15" t="s">
         <v>97</v>
       </c>
@@ -4585,7 +4577,7 @@
       </c>
       <c r="G38" s="13"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B39" s="15" t="s">
         <v>98</v>
       </c>
@@ -4603,7 +4595,7 @@
       </c>
       <c r="G39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B40" s="15" t="s">
         <v>99</v>
       </c>
@@ -4621,19 +4613,19 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B42" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B43" s="3" t="s">
         <v>0</v>
       </c>
@@ -4657,7 +4649,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A44" s="2"/>
       <c r="B44" s="15" t="s">
         <v>41</v>
@@ -4680,21 +4672,21 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="35"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="39"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+      <c r="F45" s="53"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B46" s="15" t="s">
         <v>44</v>
       </c>
@@ -4711,16 +4703,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B47" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="15" t="s">
+        <v>280</v>
+      </c>
+      <c r="D47" s="18" t="s">
         <v>281</v>
       </c>
-      <c r="D47" s="18" t="s">
-        <v>282</v>
-      </c>
       <c r="E47" s="13" t="s">
         <v>8</v>
       </c>
@@ -4729,7 +4721,7 @@
       </c>
       <c r="G47" s="13"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B48" s="15" t="s">
         <v>46</v>
       </c>
@@ -4747,18 +4739,18 @@
       </c>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="36"/>
-      <c r="E49" s="36"/>
-      <c r="F49" s="37"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="50"/>
+      <c r="E49" s="50"/>
+      <c r="F49" s="51"/>
       <c r="G49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A50" s="2"/>
       <c r="B50" s="15" t="s">
         <v>103</v>
@@ -4780,7 +4772,7 @@
       <c r="J50" s="21"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A51" s="2"/>
       <c r="B51" s="15" t="s">
         <v>104</v>
@@ -4802,7 +4794,7 @@
       <c r="J51" s="21"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B52" s="15" t="s">
         <v>105</v>
       </c>
@@ -4819,7 +4811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B53" s="15" t="s">
         <v>106</v>
       </c>
@@ -4836,7 +4828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B54" s="15" t="s">
         <v>107</v>
       </c>
@@ -4854,7 +4846,7 @@
       </c>
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B55" s="15" t="s">
         <v>108</v>
       </c>
@@ -4871,7 +4863,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B56" s="15" t="s">
         <v>109</v>
       </c>
@@ -4888,21 +4880,21 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B57" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="36"/>
-      <c r="E57" s="36"/>
-      <c r="F57" s="37"/>
+      <c r="C57" s="49"/>
+      <c r="D57" s="50"/>
+      <c r="E57" s="50"/>
+      <c r="F57" s="51"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B58" s="15" t="s">
         <v>110</v>
       </c>
@@ -4919,7 +4911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B59" s="15" t="s">
         <v>111</v>
       </c>
@@ -4936,7 +4928,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B60" s="15" t="s">
         <v>112</v>
       </c>
@@ -4953,7 +4945,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B61" s="15" t="s">
         <v>113</v>
       </c>
@@ -4970,7 +4962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B62" s="15" t="s">
         <v>114</v>
       </c>
@@ -4988,7 +4980,7 @@
       </c>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B63" s="15" t="s">
         <v>115</v>
       </c>
@@ -5006,7 +4998,7 @@
       </c>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B64" s="15" t="s">
         <v>116</v>
       </c>
@@ -5024,7 +5016,7 @@
       </c>
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B65" s="15" t="s">
         <v>117</v>
       </c>
@@ -5042,7 +5034,7 @@
       </c>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B66" s="15" t="s">
         <v>118</v>
       </c>
@@ -5060,7 +5052,7 @@
       </c>
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B67" s="15" t="s">
         <v>119</v>
       </c>
@@ -5078,7 +5070,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B68" s="15" t="s">
         <v>120</v>
       </c>
@@ -5096,7 +5088,7 @@
       </c>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B69" s="15" t="s">
         <v>121</v>
       </c>
@@ -5114,7 +5106,7 @@
       </c>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B70" s="15" t="s">
         <v>122</v>
       </c>
@@ -5132,7 +5124,7 @@
       </c>
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B71" s="15" t="s">
         <v>123</v>
       </c>
@@ -5150,7 +5142,7 @@
       </c>
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B72" s="15" t="s">
         <v>124</v>
       </c>
@@ -5168,21 +5160,21 @@
       </c>
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B73" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C73" s="35"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="37"/>
+      <c r="C73" s="49"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="50"/>
+      <c r="F73" s="51"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B74" s="15" t="s">
         <v>125</v>
       </c>
@@ -5200,7 +5192,7 @@
       </c>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B75" s="15" t="s">
         <v>126</v>
       </c>
@@ -5218,7 +5210,7 @@
       </c>
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B76" s="15" t="s">
         <v>127</v>
       </c>
@@ -5236,7 +5228,7 @@
       </c>
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B77" s="15" t="s">
         <v>128</v>
       </c>
@@ -5254,7 +5246,7 @@
       </c>
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B78" s="15" t="s">
         <v>129</v>
       </c>
@@ -5272,7 +5264,7 @@
       </c>
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B79" s="15" t="s">
         <v>130</v>
       </c>
@@ -5290,7 +5282,7 @@
       </c>
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B80" s="15" t="s">
         <v>131</v>
       </c>
@@ -5308,7 +5300,7 @@
       </c>
       <c r="G80" s="18"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B81" s="15" t="s">
         <v>132</v>
       </c>
@@ -5326,7 +5318,7 @@
       </c>
       <c r="G81" s="18"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B82" s="15" t="s">
         <v>133</v>
       </c>
@@ -5344,7 +5336,7 @@
       </c>
       <c r="G82" s="18"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B83" s="15" t="s">
         <v>134</v>
       </c>
@@ -5362,7 +5354,7 @@
       </c>
       <c r="G83" s="18"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B84" s="15" t="s">
         <v>135</v>
       </c>
@@ -5380,19 +5372,19 @@
       </c>
       <c r="G84" s="18"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B86" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
         <v>0</v>
       </c>
@@ -5416,7 +5408,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A88" s="2"/>
       <c r="B88" s="15" t="s">
         <v>51</v>
@@ -5439,13 +5431,13 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A89" s="2"/>
       <c r="B89" s="15" t="s">
         <v>52</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D89" s="8" t="s">
         <v>7</v>
@@ -5462,7 +5454,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A90" s="2"/>
       <c r="B90" s="15" t="s">
         <v>100</v>
@@ -5485,7 +5477,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A91" s="2"/>
       <c r="B91" s="15" t="s">
         <v>101</v>
@@ -5508,7 +5500,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B92" s="15" t="s">
         <v>102</v>
       </c>
@@ -5526,26 +5518,26 @@
       </c>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B95" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="40" t="s">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B96" s="54" t="s">
         <v>137</v>
       </c>
-      <c r="C96" s="40"/>
-      <c r="D96" s="40"/>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="54"/>
+      <c r="D96" s="54"/>
+    </row>
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="21" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
test du deuxieme sprint effectué
</commit_message>
<xml_diff>
--- a/annexes/Cahier_de_test.xlsx
+++ b/annexes/Cahier_de_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christophe\Documents\IUT\projet\Rosetta\git\rosetta\annexes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\rosetta\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2B165C-C9AF-4B85-8790-DE4D0E5001F1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0712B771-3087-4C63-A9EA-28EC14D28EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="2" r:id="rId1"/>
@@ -1436,7 +1436,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1553,6 +1553,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1578,7 +1581,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1876,33 +1879,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D569B6-B3CB-4EA1-907F-9E75FD9F6494}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="120.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="85.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="85.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="48" t="s">
         <v>138</v>
       </c>
       <c r="C1" s="48"/>
       <c r="D1" s="48"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="26" t="s">
         <v>267</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
         <v>15</v>
       </c>
@@ -1929,7 +1932,7 @@
       <c r="F5" s="41"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>139</v>
       </c>
@@ -1947,7 +1950,7 @@
       </c>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="30" t="s">
         <v>140</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>145</v>
       </c>
@@ -1977,11 +1980,11 @@
       <c r="E8" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F8" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F8" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
         <v>146</v>
       </c>
@@ -1994,11 +1997,11 @@
       <c r="E9" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="F9" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F9" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="30" t="s">
         <v>152</v>
       </c>
@@ -2011,11 +2014,11 @@
       <c r="E10" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="F10" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F10" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="27" t="s">
         <v>155</v>
       </c>
@@ -2028,11 +2031,11 @@
       <c r="E11" s="27" t="s">
         <v>157</v>
       </c>
-      <c r="F11" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F11" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="30" t="s">
         <v>158</v>
       </c>
@@ -2045,11 +2048,11 @@
       <c r="E12" s="30" t="s">
         <v>154</v>
       </c>
-      <c r="F12" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F12" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="27" t="s">
         <v>208</v>
@@ -2067,7 +2070,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="27" t="s">
         <v>209</v>
@@ -2081,11 +2084,11 @@
       <c r="E14" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F14" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F14" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9"/>
       <c r="B15" s="27" t="s">
         <v>210</v>
@@ -2103,7 +2106,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="27" t="s">
         <v>211</v>
@@ -2121,7 +2124,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="26" t="s">
         <v>19</v>
@@ -2131,7 +2134,7 @@
       <c r="E17" s="25"/>
       <c r="F17" s="26"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
       <c r="B18" s="27" t="s">
         <v>167</v>
@@ -2149,7 +2152,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="30" t="s">
         <v>170</v>
@@ -2167,7 +2170,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
       <c r="B20" s="27" t="s">
         <v>173</v>
@@ -2185,7 +2188,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="28" t="s">
         <v>177</v>
@@ -2203,7 +2206,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>178</v>
       </c>
@@ -2220,7 +2223,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
         <v>179</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" s="27" t="s">
         <v>204</v>
       </c>
@@ -2254,7 +2257,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>205</v>
       </c>
@@ -2271,7 +2274,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>187</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="30" t="s">
         <v>188</v>
       </c>
@@ -2305,7 +2308,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>206</v>
       </c>
@@ -2322,7 +2325,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>193</v>
       </c>
@@ -2339,7 +2342,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" s="30" t="s">
         <v>196</v>
       </c>
@@ -2356,7 +2359,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
         <v>195</v>
       </c>
@@ -2373,7 +2376,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B32" s="30" t="s">
         <v>201</v>
       </c>
@@ -2390,7 +2393,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
         <v>207</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
         <v>214</v>
       </c>
@@ -2424,7 +2427,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
         <v>217</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>219</v>
       </c>
@@ -2458,7 +2461,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="27" t="s">
         <v>223</v>
       </c>
@@ -2475,7 +2478,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="30" t="s">
         <v>224</v>
       </c>
@@ -2492,7 +2495,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>226</v>
       </c>
@@ -2509,7 +2512,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>21</v>
       </c>
@@ -2523,7 +2526,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" s="15" t="s">
         <v>233</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="15" t="s">
         <v>235</v>
       </c>
@@ -2557,7 +2560,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="15" t="s">
         <v>238</v>
       </c>
@@ -2574,7 +2577,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" s="15" t="s">
         <v>239</v>
       </c>
@@ -2591,7 +2594,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" s="27" t="s">
         <v>243</v>
       </c>
@@ -2608,7 +2611,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="30" t="s">
         <v>244</v>
       </c>
@@ -2625,7 +2628,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
         <v>247</v>
       </c>
@@ -2642,7 +2645,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="s">
         <v>250</v>
       </c>
@@ -2659,7 +2662,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B49" s="15" t="s">
         <v>252</v>
       </c>
@@ -2676,7 +2679,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B50" s="27" t="s">
         <v>256</v>
       </c>
@@ -2693,7 +2696,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B51" s="30" t="s">
         <v>260</v>
       </c>
@@ -2710,7 +2713,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B52" s="27" t="s">
         <v>261</v>
       </c>
@@ -2727,7 +2730,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B53" s="30" t="s">
         <v>262</v>
       </c>
@@ -2744,7 +2747,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
         <v>263</v>
       </c>
@@ -2761,18 +2764,18 @@
         <v>331</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F55" s="43"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
       <c r="F56" s="43"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B58" s="26" t="s">
         <v>267</v>
       </c>
@@ -2789,7 +2792,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B59" s="34" t="s">
         <v>272</v>
       </c>
@@ -2806,7 +2809,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B60" s="34" t="s">
         <v>273</v>
       </c>
@@ -2823,7 +2826,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B61" s="26" t="s">
         <v>43</v>
       </c>
@@ -2832,7 +2835,7 @@
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
         <v>276</v>
       </c>
@@ -2849,7 +2852,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="s">
         <v>279</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>284</v>
       </c>
@@ -2883,7 +2886,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
         <v>15</v>
       </c>
@@ -2892,7 +2895,7 @@
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
         <v>293</v>
       </c>
@@ -2909,7 +2912,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B67" s="30" t="s">
         <v>294</v>
       </c>
@@ -2926,7 +2929,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B68" s="27" t="s">
         <v>295</v>
       </c>
@@ -2939,11 +2942,11 @@
       <c r="E68" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="F68" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F68" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B69" s="28" t="s">
         <v>296</v>
       </c>
@@ -2960,7 +2963,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B70" s="28" t="s">
         <v>297</v>
       </c>
@@ -2977,7 +2980,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B71" s="27" t="s">
         <v>288</v>
       </c>
@@ -2994,7 +2997,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B72" s="28" t="s">
         <v>289</v>
       </c>
@@ -3011,7 +3014,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B73" s="28" t="s">
         <v>291</v>
       </c>
@@ -3028,7 +3031,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B74" s="27" t="s">
         <v>299</v>
       </c>
@@ -3045,7 +3048,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
         <v>300</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
         <v>301</v>
       </c>
@@ -3079,7 +3082,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B77" s="27" t="s">
         <v>302</v>
       </c>
@@ -3096,7 +3099,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B78" s="26" t="s">
         <v>19</v>
       </c>
@@ -3105,7 +3108,7 @@
       <c r="E78" s="25"/>
       <c r="F78" s="26"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B79" s="27" t="s">
         <v>167</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B80" s="30" t="s">
         <v>170</v>
       </c>
@@ -3139,7 +3142,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B81" s="27" t="s">
         <v>173</v>
       </c>
@@ -3156,7 +3159,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B82" s="28" t="s">
         <v>177</v>
       </c>
@@ -3173,7 +3176,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B83" s="27" t="s">
         <v>178</v>
       </c>
@@ -3190,7 +3193,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B84" s="28" t="s">
         <v>179</v>
       </c>
@@ -3207,7 +3210,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B85" s="27" t="s">
         <v>204</v>
       </c>
@@ -3224,7 +3227,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B86" s="15" t="s">
         <v>205</v>
       </c>
@@ -3241,7 +3244,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B87" s="27" t="s">
         <v>187</v>
       </c>
@@ -3258,7 +3261,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B88" s="30" t="s">
         <v>188</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B89" s="15" t="s">
         <v>206</v>
       </c>
@@ -3292,7 +3295,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B90" s="27" t="s">
         <v>193</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B91" s="30" t="s">
         <v>196</v>
       </c>
@@ -3326,7 +3329,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B92" s="27" t="s">
         <v>195</v>
       </c>
@@ -3343,7 +3346,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B93" s="30" t="s">
         <v>201</v>
       </c>
@@ -3360,7 +3363,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
         <v>207</v>
       </c>
@@ -3377,7 +3380,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B95" s="15" t="s">
         <v>214</v>
       </c>
@@ -3394,7 +3397,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B96" s="15" t="s">
         <v>217</v>
       </c>
@@ -3411,7 +3414,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="15" t="s">
         <v>219</v>
       </c>
@@ -3428,7 +3431,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="27" t="s">
         <v>223</v>
       </c>
@@ -3445,7 +3448,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="30" t="s">
         <v>224</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="15" t="s">
         <v>226</v>
       </c>
@@ -3479,7 +3482,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
         <v>21</v>
       </c>
@@ -3488,7 +3491,7 @@
       <c r="E101" s="50"/>
       <c r="F101" s="51"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="15" t="s">
         <v>233</v>
       </c>
@@ -3505,7 +3508,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="15" t="s">
         <v>235</v>
       </c>
@@ -3522,7 +3525,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="s">
         <v>238</v>
       </c>
@@ -3539,7 +3542,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
         <v>239</v>
       </c>
@@ -3556,7 +3559,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="27" t="s">
         <v>243</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="30" t="s">
         <v>244</v>
       </c>
@@ -3590,7 +3593,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="s">
         <v>247</v>
       </c>
@@ -3607,7 +3610,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="s">
         <v>250</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="s">
         <v>252</v>
       </c>
@@ -3641,7 +3644,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="27" t="s">
         <v>256</v>
       </c>
@@ -3658,7 +3661,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B112" s="30" t="s">
         <v>260</v>
       </c>
@@ -3675,7 +3678,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="27" t="s">
         <v>261</v>
       </c>
@@ -3692,7 +3695,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B114" s="30" t="s">
         <v>262</v>
       </c>
@@ -3709,7 +3712,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="15" t="s">
         <v>263</v>
       </c>
@@ -3722,16 +3725,16 @@
       <c r="E115" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F115" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F115" s="56" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B117" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B118" s="26" t="s">
         <v>267</v>
       </c>
@@ -3748,7 +3751,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B119" s="27" t="s">
         <v>305</v>
       </c>
@@ -3765,7 +3768,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B120" s="28" t="s">
         <v>306</v>
       </c>
@@ -3782,7 +3785,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B121" s="30" t="s">
         <v>310</v>
       </c>
@@ -3799,7 +3802,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B122" s="15" t="s">
         <v>313</v>
       </c>
@@ -3816,7 +3819,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B123" s="27" t="s">
         <v>318</v>
       </c>
@@ -3833,7 +3836,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B124" s="28" t="s">
         <v>319</v>
       </c>
@@ -3850,7 +3853,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B125" s="30" t="s">
         <v>320</v>
       </c>
@@ -3867,7 +3870,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B126" s="27" t="s">
         <v>323</v>
       </c>
@@ -3884,7 +3887,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B127" s="30" t="s">
         <v>325</v>
       </c>
@@ -3901,7 +3904,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B128" s="15" t="s">
         <v>329</v>
       </c>
@@ -3914,7 +3917,7 @@
       <c r="E128" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="F128" s="42" t="s">
+      <c r="F128" s="56" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3938,30 +3941,30 @@
       <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="127.109375" customWidth="1"/>
+    <col min="3" max="3" width="127.140625" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="26.109375" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="43.5546875" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="43.5703125" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
       <c r="B1" s="55" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="55"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
@@ -3980,7 +3983,7 @@
       <c r="G4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
@@ -3991,7 +3994,7 @@
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="15" t="s">
         <v>23</v>
@@ -4013,7 +4016,7 @@
       <c r="J6" s="21"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="15" t="s">
         <v>24</v>
@@ -4035,7 +4038,7 @@
       <c r="J7" s="21"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
         <v>25</v>
       </c>
@@ -4052,7 +4055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="15" t="s">
         <v>58</v>
       </c>
@@ -4087,7 +4090,7 @@
       </c>
       <c r="G10" s="13"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
         <v>59</v>
       </c>
@@ -4104,7 +4107,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="15" t="s">
         <v>60</v>
       </c>
@@ -4121,7 +4124,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
@@ -4135,7 +4138,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="15" t="s">
         <v>27</v>
       </c>
@@ -4152,7 +4155,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B15" s="15" t="s">
         <v>28</v>
       </c>
@@ -4169,7 +4172,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
@@ -4186,7 +4189,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="15" t="s">
         <v>30</v>
       </c>
@@ -4203,7 +4206,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="15" t="s">
         <v>31</v>
       </c>
@@ -4221,7 +4224,7 @@
       </c>
       <c r="G18" s="13"/>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="15" t="s">
         <v>32</v>
       </c>
@@ -4239,7 +4242,7 @@
       </c>
       <c r="G19" s="13"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="15" t="s">
         <v>74</v>
       </c>
@@ -4257,7 +4260,7 @@
       </c>
       <c r="G20" s="13"/>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="15" t="s">
         <v>75</v>
       </c>
@@ -4275,7 +4278,7 @@
       </c>
       <c r="G21" s="13"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>76</v>
       </c>
@@ -4293,7 +4296,7 @@
       </c>
       <c r="G22" s="13"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>77</v>
       </c>
@@ -4311,7 +4314,7 @@
       </c>
       <c r="G23" s="13"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
         <v>78</v>
       </c>
@@ -4329,7 +4332,7 @@
       </c>
       <c r="G24" s="13"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>79</v>
       </c>
@@ -4347,7 +4350,7 @@
       </c>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>80</v>
       </c>
@@ -4365,7 +4368,7 @@
       </c>
       <c r="G26" s="13"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>81</v>
       </c>
@@ -4383,7 +4386,7 @@
       </c>
       <c r="G27" s="13"/>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>82</v>
       </c>
@@ -4401,7 +4404,7 @@
       </c>
       <c r="G28" s="13"/>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>21</v>
       </c>
@@ -4415,7 +4418,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>33</v>
       </c>
@@ -4433,7 +4436,7 @@
       </c>
       <c r="G30" s="13"/>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
         <v>34</v>
       </c>
@@ -4451,7 +4454,7 @@
       </c>
       <c r="G31" s="13"/>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
         <v>35</v>
       </c>
@@ -4469,7 +4472,7 @@
       </c>
       <c r="G32" s="13"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B33" s="15" t="s">
         <v>37</v>
       </c>
@@ -4487,7 +4490,7 @@
       </c>
       <c r="G33" s="13"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B34" s="15" t="s">
         <v>38</v>
       </c>
@@ -4505,7 +4508,7 @@
       </c>
       <c r="G34" s="13"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B35" s="15" t="s">
         <v>94</v>
       </c>
@@ -4523,7 +4526,7 @@
       </c>
       <c r="G35" s="13"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B36" s="15" t="s">
         <v>95</v>
       </c>
@@ -4541,7 +4544,7 @@
       </c>
       <c r="G36" s="13"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B37" s="15" t="s">
         <v>96</v>
       </c>
@@ -4559,7 +4562,7 @@
       </c>
       <c r="G37" s="13"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B38" s="15" t="s">
         <v>97</v>
       </c>
@@ -4577,7 +4580,7 @@
       </c>
       <c r="G38" s="13"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B39" s="15" t="s">
         <v>98</v>
       </c>
@@ -4595,7 +4598,7 @@
       </c>
       <c r="G39" s="13"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="15" t="s">
         <v>99</v>
       </c>
@@ -4613,19 +4616,19 @@
       </c>
       <c r="G40" s="13"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B42" s="16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>0</v>
       </c>
@@ -4649,7 +4652,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="15" t="s">
         <v>41</v>
@@ -4672,7 +4675,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
@@ -4686,7 +4689,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B46" s="15" t="s">
         <v>44</v>
       </c>
@@ -4703,7 +4706,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B47" s="15" t="s">
         <v>45</v>
       </c>
@@ -4721,7 +4724,7 @@
       </c>
       <c r="G47" s="13"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B48" s="15" t="s">
         <v>46</v>
       </c>
@@ -4739,7 +4742,7 @@
       </c>
       <c r="G48" s="13"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>15</v>
       </c>
@@ -4750,7 +4753,7 @@
       <c r="G49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="15" t="s">
         <v>103</v>
@@ -4772,7 +4775,7 @@
       <c r="J50" s="21"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="15" t="s">
         <v>104</v>
@@ -4794,7 +4797,7 @@
       <c r="J51" s="21"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="15" t="s">
         <v>105</v>
       </c>
@@ -4811,7 +4814,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="15" t="s">
         <v>106</v>
       </c>
@@ -4828,7 +4831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="15" t="s">
         <v>107</v>
       </c>
@@ -4846,7 +4849,7 @@
       </c>
       <c r="G54" s="13"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B55" s="15" t="s">
         <v>108</v>
       </c>
@@ -4863,7 +4866,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B56" s="15" t="s">
         <v>109</v>
       </c>
@@ -4880,7 +4883,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>19</v>
       </c>
@@ -4894,7 +4897,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" s="15" t="s">
         <v>110</v>
       </c>
@@ -4911,7 +4914,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" s="15" t="s">
         <v>111</v>
       </c>
@@ -4928,7 +4931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" s="15" t="s">
         <v>112</v>
       </c>
@@ -4945,7 +4948,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B61" s="15" t="s">
         <v>113</v>
       </c>
@@ -4962,7 +4965,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B62" s="15" t="s">
         <v>114</v>
       </c>
@@ -4980,7 +4983,7 @@
       </c>
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" s="15" t="s">
         <v>115</v>
       </c>
@@ -4998,7 +5001,7 @@
       </c>
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" s="15" t="s">
         <v>116</v>
       </c>
@@ -5016,7 +5019,7 @@
       </c>
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B65" s="15" t="s">
         <v>117</v>
       </c>
@@ -5034,7 +5037,7 @@
       </c>
       <c r="G65" s="13"/>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B66" s="15" t="s">
         <v>118</v>
       </c>
@@ -5052,7 +5055,7 @@
       </c>
       <c r="G66" s="13"/>
     </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B67" s="15" t="s">
         <v>119</v>
       </c>
@@ -5070,7 +5073,7 @@
       </c>
       <c r="G67" s="13"/>
     </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="15" t="s">
         <v>120</v>
       </c>
@@ -5088,7 +5091,7 @@
       </c>
       <c r="G68" s="13"/>
     </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="15" t="s">
         <v>121</v>
       </c>
@@ -5106,7 +5109,7 @@
       </c>
       <c r="G69" s="13"/>
     </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B70" s="15" t="s">
         <v>122</v>
       </c>
@@ -5124,7 +5127,7 @@
       </c>
       <c r="G70" s="13"/>
     </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
         <v>123</v>
       </c>
@@ -5142,7 +5145,7 @@
       </c>
       <c r="G71" s="13"/>
     </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="15" t="s">
         <v>124</v>
       </c>
@@ -5160,7 +5163,7 @@
       </c>
       <c r="G72" s="13"/>
     </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
         <v>21</v>
       </c>
@@ -5174,7 +5177,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B74" s="15" t="s">
         <v>125</v>
       </c>
@@ -5192,7 +5195,7 @@
       </c>
       <c r="G74" s="13"/>
     </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B75" s="15" t="s">
         <v>126</v>
       </c>
@@ -5210,7 +5213,7 @@
       </c>
       <c r="G75" s="13"/>
     </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="15" t="s">
         <v>127</v>
       </c>
@@ -5228,7 +5231,7 @@
       </c>
       <c r="G76" s="13"/>
     </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="s">
         <v>128</v>
       </c>
@@ -5246,7 +5249,7 @@
       </c>
       <c r="G77" s="13"/>
     </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B78" s="15" t="s">
         <v>129</v>
       </c>
@@ -5264,7 +5267,7 @@
       </c>
       <c r="G78" s="13"/>
     </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B79" s="15" t="s">
         <v>130</v>
       </c>
@@ -5282,7 +5285,7 @@
       </c>
       <c r="G79" s="13"/>
     </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B80" s="15" t="s">
         <v>131</v>
       </c>
@@ -5300,7 +5303,7 @@
       </c>
       <c r="G80" s="18"/>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B81" s="15" t="s">
         <v>132</v>
       </c>
@@ -5318,7 +5321,7 @@
       </c>
       <c r="G81" s="18"/>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B82" s="15" t="s">
         <v>133</v>
       </c>
@@ -5336,7 +5339,7 @@
       </c>
       <c r="G82" s="18"/>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B83" s="15" t="s">
         <v>134</v>
       </c>
@@ -5354,7 +5357,7 @@
       </c>
       <c r="G83" s="18"/>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B84" s="15" t="s">
         <v>135</v>
       </c>
@@ -5372,19 +5375,19 @@
       </c>
       <c r="G84" s="18"/>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
       <c r="F85" s="2"/>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B86" s="16" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B87" s="3" t="s">
         <v>0</v>
       </c>
@@ -5408,7 +5411,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="15" t="s">
         <v>51</v>
@@ -5431,7 +5434,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
       <c r="B89" s="15" t="s">
         <v>52</v>
@@ -5454,7 +5457,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="15" t="s">
         <v>100</v>
@@ -5477,7 +5480,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="15" t="s">
         <v>101</v>
@@ -5500,7 +5503,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" s="15" t="s">
         <v>102</v>
       </c>
@@ -5518,26 +5521,26 @@
       </c>
       <c r="G92" s="22"/>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B93" s="2"/>
       <c r="C93" s="2"/>
       <c r="D93" s="13"/>
       <c r="E93" s="13"/>
       <c r="F93" s="2"/>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B95" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" s="54" t="s">
         <v>137</v>
       </c>
       <c r="C96" s="54"/>
       <c r="D96" s="54"/>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="21" t="s">
         <v>136</v>
       </c>

</xml_diff>

<commit_message>
mise a jour du cahier de test
</commit_message>
<xml_diff>
--- a/annexes/Cahier_de_test.xlsx
+++ b/annexes/Cahier_de_test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Travail\Projet\rosetta\annexes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0712B771-3087-4C63-A9EA-28EC14D28EEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{809A3CA1-26A6-491D-A1CD-113928E6ECD3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tests" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="982" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="370">
   <si>
     <t>Code</t>
   </si>
@@ -1115,7 +1115,121 @@
     <t>Synchronisation des donnée entre la tablette et le site web</t>
   </si>
   <si>
-    <t>Non testé</t>
+    <t>Test PAS OK</t>
+  </si>
+  <si>
+    <t>ExiWebScenario1 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario1 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario2 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario2 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario3 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario3 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario4 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario5 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario6 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario6 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario7 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario8 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario8 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario9 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario9 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario10 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario11 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario12 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario13 T</t>
+  </si>
+  <si>
+    <t>ExiWebScenario14 T1</t>
+  </si>
+  <si>
+    <t>ExiWebScenario14 T2</t>
+  </si>
+  <si>
+    <t>ExiWebScenario15 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis1 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis2 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis3 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis4 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis5 T1</t>
+  </si>
+  <si>
+    <t>ExiWebDevis5 T2</t>
+  </si>
+  <si>
+    <t>ExiWebDevis6 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis7 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis8 T</t>
+  </si>
+  <si>
+    <t>ExiWebDevis9 T1</t>
+  </si>
+  <si>
+    <t>ExiWebDevis9 T2</t>
+  </si>
+  <si>
+    <t>ExiWebDevis10 T1</t>
+  </si>
+  <si>
+    <t>ExiWebDevis10 T2</t>
+  </si>
+  <si>
+    <t>ExiWebDevis11 T</t>
+  </si>
+  <si>
+    <t>Test IMPOSSIBLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test impossible car les spécifications du site ont changé entre temps</t>
   </si>
 </sst>
 </file>
@@ -1436,7 +1550,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1527,6 +1641,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1879,8 +1996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D569B6-B3CB-4EA1-907F-9E75FD9F6494}">
   <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1890,15 +2007,16 @@
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="120.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="49" t="s">
         <v>138</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -1945,8 +2063,8 @@
       <c r="E6" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="F6" s="42" t="s">
-        <v>331</v>
+      <c r="F6" s="45" t="s">
+        <v>304</v>
       </c>
       <c r="G6" s="8"/>
     </row>
@@ -1963,8 +2081,8 @@
       <c r="E7" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="F7" s="42" t="s">
-        <v>331</v>
+      <c r="F7" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2066,8 +2184,8 @@
       <c r="E13" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="F13" s="42" t="s">
-        <v>331</v>
+      <c r="F13" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2102,8 +2220,8 @@
       <c r="E15" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="F15" s="42" t="s">
-        <v>331</v>
+      <c r="F15" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2120,8 +2238,8 @@
       <c r="E16" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="F16" s="42" t="s">
-        <v>331</v>
+      <c r="F16" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2148,8 +2266,8 @@
       <c r="E18" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="F18" s="42" t="s">
-        <v>331</v>
+      <c r="F18" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2184,8 +2302,8 @@
       <c r="E20" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="F20" s="42" t="s">
-        <v>331</v>
+      <c r="F20" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -2219,8 +2337,8 @@
       <c r="E22" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="42" t="s">
-        <v>331</v>
+      <c r="F22" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2270,8 +2388,8 @@
       <c r="E25" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F25" s="42" t="s">
-        <v>331</v>
+      <c r="F25" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -2321,8 +2439,8 @@
       <c r="E28" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F28" s="42" t="s">
-        <v>331</v>
+      <c r="F28" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2338,8 +2456,8 @@
       <c r="E29" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="F29" s="42" t="s">
-        <v>331</v>
+      <c r="F29" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2355,8 +2473,8 @@
       <c r="E30" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="F30" s="42" t="s">
-        <v>331</v>
+      <c r="F30" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2423,8 +2541,8 @@
       <c r="E34" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="F34" s="42" t="s">
-        <v>331</v>
+      <c r="F34" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
@@ -2440,8 +2558,8 @@
       <c r="E35" s="15" t="s">
         <v>216</v>
       </c>
-      <c r="F35" s="42" t="s">
-        <v>331</v>
+      <c r="F35" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -2457,8 +2575,8 @@
       <c r="E36" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="F36" s="42" t="s">
-        <v>331</v>
+      <c r="F36" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
@@ -2474,8 +2592,8 @@
       <c r="E37" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="F37" s="42" t="s">
-        <v>331</v>
+      <c r="F37" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
@@ -2508,18 +2626,18 @@
       <c r="E39" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="F39" s="42" t="s">
-        <v>331</v>
+      <c r="F39" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C40" s="49"/>
-      <c r="D40" s="50"/>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="52"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
@@ -2590,8 +2708,8 @@
       <c r="E44" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="F44" s="42" t="s">
-        <v>331</v>
+      <c r="F44" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -2641,8 +2759,8 @@
       <c r="E47" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="F47" s="42" t="s">
-        <v>331</v>
+      <c r="F47" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
@@ -2658,8 +2776,8 @@
       <c r="E48" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="F48" s="42" t="s">
-        <v>331</v>
+      <c r="F48" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
@@ -2675,8 +2793,8 @@
       <c r="E49" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="F49" s="42" t="s">
-        <v>331</v>
+      <c r="F49" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
@@ -2760,7 +2878,7 @@
       <c r="E54" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F54" s="42" t="s">
+      <c r="F54" s="57" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2805,8 +2923,8 @@
       <c r="E59" s="34" t="s">
         <v>277</v>
       </c>
-      <c r="F59" s="42" t="s">
-        <v>331</v>
+      <c r="F59" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
@@ -2822,8 +2940,8 @@
       <c r="E60" s="34" t="s">
         <v>275</v>
       </c>
-      <c r="F60" s="42" t="s">
-        <v>331</v>
+      <c r="F60" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
@@ -2882,11 +3000,11 @@
       <c r="E64" t="s">
         <v>286</v>
       </c>
-      <c r="F64" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F64" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="26" t="s">
         <v>15</v>
       </c>
@@ -2895,7 +3013,7 @@
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
     </row>
-    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="27" t="s">
         <v>293</v>
       </c>
@@ -2908,11 +3026,11 @@
       <c r="E66" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="F66" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F66" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="30" t="s">
         <v>294</v>
       </c>
@@ -2925,11 +3043,11 @@
       <c r="E67" s="30" t="s">
         <v>144</v>
       </c>
-      <c r="F67" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F67" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B68" s="27" t="s">
         <v>295</v>
       </c>
@@ -2946,7 +3064,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="28" t="s">
         <v>296</v>
       </c>
@@ -2963,7 +3081,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="28" t="s">
         <v>297</v>
       </c>
@@ -2980,7 +3098,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="27" t="s">
         <v>288</v>
       </c>
@@ -2993,11 +3111,11 @@
       <c r="E71" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F71" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F71" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B72" s="28" t="s">
         <v>289</v>
       </c>
@@ -3014,7 +3132,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="28" t="s">
         <v>291</v>
       </c>
@@ -3031,7 +3149,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="27" t="s">
         <v>299</v>
       </c>
@@ -3044,11 +3162,11 @@
       <c r="E74" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="F74" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F74" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
         <v>300</v>
       </c>
@@ -3061,11 +3179,11 @@
       <c r="E75" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F75" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F75" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B76" s="27" t="s">
         <v>301</v>
       </c>
@@ -3081,8 +3199,9 @@
       <c r="F76" s="42" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="27" t="s">
         <v>302</v>
       </c>
@@ -3098,8 +3217,9 @@
       <c r="F77" s="42" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="H77" s="43"/>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="26" t="s">
         <v>19</v>
       </c>
@@ -3108,9 +3228,9 @@
       <c r="E78" s="25"/>
       <c r="F78" s="26"/>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="27" t="s">
-        <v>167</v>
+        <v>332</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>11</v>
@@ -3121,13 +3241,13 @@
       <c r="E79" s="27" t="s">
         <v>169</v>
       </c>
-      <c r="F79" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="30" t="s">
-        <v>170</v>
+      <c r="F79" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="27" t="s">
+        <v>333</v>
       </c>
       <c r="C80" s="30" t="s">
         <v>142</v>
@@ -3142,9 +3262,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" s="27" t="s">
-        <v>173</v>
+        <v>334</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>11</v>
@@ -3155,13 +3275,16 @@
       <c r="E81" s="27" t="s">
         <v>175</v>
       </c>
-      <c r="F81" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="28" t="s">
-        <v>177</v>
+      <c r="F81" s="48" t="s">
+        <v>368</v>
+      </c>
+      <c r="G81" s="44" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="27" t="s">
+        <v>335</v>
       </c>
       <c r="C82" s="30" t="s">
         <v>142</v>
@@ -3172,13 +3295,13 @@
       <c r="E82" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="F82" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F82" s="48" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" s="27" t="s">
-        <v>178</v>
+        <v>336</v>
       </c>
       <c r="C83" s="27" t="s">
         <v>11</v>
@@ -3189,13 +3312,13 @@
       <c r="E83" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F83" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="28" t="s">
-        <v>179</v>
+      <c r="F83" s="48" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="27" t="s">
+        <v>337</v>
       </c>
       <c r="C84" s="28" t="s">
         <v>142</v>
@@ -3206,13 +3329,13 @@
       <c r="E84" s="28" t="s">
         <v>151</v>
       </c>
-      <c r="F84" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F84" s="48" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" s="27" t="s">
-        <v>204</v>
+        <v>338</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>11</v>
@@ -3223,13 +3346,13 @@
       <c r="E85" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="F85" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F85" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" s="15" t="s">
-        <v>205</v>
+        <v>339</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>11</v>
@@ -3240,13 +3363,13 @@
       <c r="E86" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="F86" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F86" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" s="27" t="s">
-        <v>187</v>
+        <v>340</v>
       </c>
       <c r="C87" s="27" t="s">
         <v>11</v>
@@ -3257,13 +3380,13 @@
       <c r="E87" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F87" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="30" t="s">
-        <v>188</v>
+      <c r="F87" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B88" s="27" t="s">
+        <v>341</v>
       </c>
       <c r="C88" s="30" t="s">
         <v>142</v>
@@ -3278,9 +3401,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="89" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" s="15" t="s">
-        <v>206</v>
+        <v>342</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>11</v>
@@ -3291,13 +3414,13 @@
       <c r="E89" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="F89" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F89" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" s="27" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>11</v>
@@ -3312,9 +3435,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="30" t="s">
-        <v>196</v>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B91" s="27" t="s">
+        <v>344</v>
       </c>
       <c r="C91" s="30" t="s">
         <v>142</v>
@@ -3329,9 +3452,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" s="27" t="s">
-        <v>195</v>
+        <v>345</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>11</v>
@@ -3346,9 +3469,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="30" t="s">
-        <v>201</v>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B93" s="27" t="s">
+        <v>346</v>
       </c>
       <c r="C93" s="30" t="s">
         <v>142</v>
@@ -3363,9 +3486,9 @@
         <v>331</v>
       </c>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" s="15" t="s">
-        <v>207</v>
+        <v>347</v>
       </c>
       <c r="C94" s="15" t="s">
         <v>11</v>
@@ -3376,13 +3499,13 @@
       <c r="E94" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="F94" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F94" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" s="15" t="s">
-        <v>214</v>
+        <v>348</v>
       </c>
       <c r="C95" s="15" t="s">
         <v>11</v>
@@ -3393,13 +3516,13 @@
       <c r="E95" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="F95" s="42" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F95" s="45" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" s="15" t="s">
-        <v>217</v>
+        <v>349</v>
       </c>
       <c r="C96" s="15" t="s">
         <v>11</v>
@@ -3416,7 +3539,7 @@
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B97" s="15" t="s">
-        <v>219</v>
+        <v>350</v>
       </c>
       <c r="C97" s="15" t="s">
         <v>11</v>
@@ -3427,13 +3550,13 @@
       <c r="E97" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="F97" s="42" t="s">
-        <v>331</v>
+      <c r="F97" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B98" s="27" t="s">
-        <v>223</v>
+        <v>351</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>11</v>
@@ -3444,13 +3567,13 @@
       <c r="E98" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="F98" s="42" t="s">
-        <v>331</v>
+      <c r="F98" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B99" s="30" t="s">
-        <v>224</v>
+        <v>352</v>
       </c>
       <c r="C99" s="30" t="s">
         <v>142</v>
@@ -3467,7 +3590,7 @@
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B100" s="15" t="s">
-        <v>226</v>
+        <v>353</v>
       </c>
       <c r="C100" s="15" t="s">
         <v>11</v>
@@ -3486,14 +3609,14 @@
       <c r="B101" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C101" s="49"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="50"/>
-      <c r="F101" s="51"/>
+      <c r="C101" s="50"/>
+      <c r="D101" s="51"/>
+      <c r="E101" s="51"/>
+      <c r="F101" s="52"/>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="15" t="s">
-        <v>233</v>
+        <v>354</v>
       </c>
       <c r="C102" s="15" t="s">
         <v>11</v>
@@ -3504,13 +3627,13 @@
       <c r="E102" s="32" t="s">
         <v>232</v>
       </c>
-      <c r="F102" s="42" t="s">
-        <v>331</v>
+      <c r="F102" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="103" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B103" s="15" t="s">
-        <v>235</v>
+        <v>355</v>
       </c>
       <c r="C103" s="15" t="s">
         <v>11</v>
@@ -3521,13 +3644,13 @@
       <c r="E103" s="32" t="s">
         <v>236</v>
       </c>
-      <c r="F103" s="42" t="s">
-        <v>331</v>
+      <c r="F103" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="104" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="s">
-        <v>238</v>
+        <v>356</v>
       </c>
       <c r="C104" s="15" t="s">
         <v>11</v>
@@ -3538,13 +3661,13 @@
       <c r="E104" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="F104" s="42" t="s">
-        <v>331</v>
+      <c r="F104" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="105" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B105" s="15" t="s">
-        <v>239</v>
+        <v>357</v>
       </c>
       <c r="C105" s="15" t="s">
         <v>11</v>
@@ -3555,13 +3678,13 @@
       <c r="E105" s="32" t="s">
         <v>241</v>
       </c>
-      <c r="F105" s="42" t="s">
-        <v>331</v>
+      <c r="F105" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="106" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B106" s="27" t="s">
-        <v>243</v>
+        <v>358</v>
       </c>
       <c r="C106" s="27" t="s">
         <v>11</v>
@@ -3572,13 +3695,13 @@
       <c r="E106" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="F106" s="42" t="s">
-        <v>331</v>
+      <c r="F106" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="107" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B107" s="30" t="s">
-        <v>244</v>
+        <v>359</v>
       </c>
       <c r="C107" s="30" t="s">
         <v>142</v>
@@ -3589,13 +3712,13 @@
       <c r="E107" s="30" t="s">
         <v>172</v>
       </c>
-      <c r="F107" s="42" t="s">
-        <v>331</v>
+      <c r="F107" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="108" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B108" s="15" t="s">
-        <v>247</v>
+        <v>360</v>
       </c>
       <c r="C108" s="15" t="s">
         <v>11</v>
@@ -3606,13 +3729,13 @@
       <c r="E108" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="F108" s="42" t="s">
-        <v>331</v>
+      <c r="F108" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="109" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B109" s="15" t="s">
-        <v>250</v>
+        <v>361</v>
       </c>
       <c r="C109" s="15" t="s">
         <v>11</v>
@@ -3623,13 +3746,13 @@
       <c r="E109" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="F109" s="42" t="s">
-        <v>331</v>
+      <c r="F109" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="110" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B110" s="15" t="s">
-        <v>252</v>
+        <v>362</v>
       </c>
       <c r="C110" s="15" t="s">
         <v>11</v>
@@ -3640,13 +3763,13 @@
       <c r="E110" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="F110" s="42" t="s">
-        <v>331</v>
+      <c r="F110" s="48" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="111" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B111" s="27" t="s">
-        <v>256</v>
+        <v>363</v>
       </c>
       <c r="C111" s="27" t="s">
         <v>11</v>
@@ -3657,13 +3780,13 @@
       <c r="E111" s="33" t="s">
         <v>258</v>
       </c>
-      <c r="F111" s="42" t="s">
-        <v>331</v>
+      <c r="F111" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="112" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B112" s="30" t="s">
-        <v>260</v>
+      <c r="B112" s="27" t="s">
+        <v>364</v>
       </c>
       <c r="C112" s="30" t="s">
         <v>142</v>
@@ -3680,7 +3803,7 @@
     </row>
     <row r="113" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B113" s="27" t="s">
-        <v>261</v>
+        <v>365</v>
       </c>
       <c r="C113" s="27" t="s">
         <v>11</v>
@@ -3691,13 +3814,13 @@
       <c r="E113" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="F113" s="42" t="s">
-        <v>331</v>
+      <c r="F113" s="45" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="114" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B114" s="30" t="s">
-        <v>262</v>
+      <c r="B114" s="27" t="s">
+        <v>366</v>
       </c>
       <c r="C114" s="30" t="s">
         <v>142</v>
@@ -3714,7 +3837,7 @@
     </row>
     <row r="115" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B115" s="15" t="s">
-        <v>263</v>
+        <v>367</v>
       </c>
       <c r="C115" s="15" t="s">
         <v>11</v>
@@ -3725,8 +3848,8 @@
       <c r="E115" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="F115" s="56" t="s">
-        <v>331</v>
+      <c r="F115" s="40" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="117" spans="2:6" x14ac:dyDescent="0.25">
@@ -3917,7 +4040,7 @@
       <c r="E128" s="32" t="s">
         <v>330</v>
       </c>
-      <c r="F128" s="56" t="s">
+      <c r="F128" s="42" t="s">
         <v>331</v>
       </c>
     </row>
@@ -3954,10 +4077,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="55"/>
+      <c r="C1" s="56"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
@@ -3987,10 +4110,10 @@
       <c r="B5" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="51"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="1"/>
       <c r="K5" s="1"/>
     </row>
@@ -4128,10 +4251,10 @@
       <c r="B13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="50"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="51"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="52"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -4408,10 +4531,10 @@
       <c r="B29" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="49"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="51"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
@@ -4679,10 +4802,10 @@
       <c r="B45" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
-      <c r="F45" s="53"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="53"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="54"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
@@ -4746,10 +4869,10 @@
       <c r="B49" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="49"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="50"/>
-      <c r="F49" s="51"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="51"/>
+      <c r="E49" s="51"/>
+      <c r="F49" s="52"/>
       <c r="G49" s="1"/>
       <c r="K49" s="1"/>
     </row>
@@ -4887,10 +5010,10 @@
       <c r="B57" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="49"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="F57" s="51"/>
+      <c r="C57" s="50"/>
+      <c r="D57" s="51"/>
+      <c r="E57" s="51"/>
+      <c r="F57" s="52"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
@@ -5167,10 +5290,10 @@
       <c r="B73" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C73" s="49"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="51"/>
+      <c r="C73" s="50"/>
+      <c r="D73" s="51"/>
+      <c r="E73" s="51"/>
+      <c r="F73" s="52"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
@@ -5534,11 +5657,11 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B96" s="54" t="s">
+      <c r="B96" s="55" t="s">
         <v>137</v>
       </c>
-      <c r="C96" s="54"/>
-      <c r="D96" s="54"/>
+      <c r="C96" s="55"/>
+      <c r="D96" s="55"/>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B97" s="21" t="s">

</xml_diff>